<commit_message>
Some edits on the graphical part of the total time
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>Worked by:</t>
   </si>
@@ -52,83 +52,107 @@
     <t>Georgi</t>
   </si>
   <si>
-    <t>Date started and finished</t>
-  </si>
-  <si>
-    <t>26.02-26.02</t>
-  </si>
-  <si>
-    <t>25.02.-25.02.</t>
-  </si>
-  <si>
     <t>Minutes worked</t>
   </si>
   <si>
-    <t>23.02.-</t>
-  </si>
-  <si>
     <t>Project plan v2</t>
   </si>
   <si>
-    <t>04.03.-</t>
-  </si>
-  <si>
-    <t>21.02-02.03</t>
-  </si>
-  <si>
     <t>Group logo</t>
   </si>
   <si>
     <t>Mikaeil</t>
   </si>
   <si>
-    <t xml:space="preserve">21.02. - </t>
-  </si>
-  <si>
     <t>Website design/code</t>
   </si>
   <si>
     <t>Angel</t>
   </si>
   <si>
-    <t>07.03-</t>
-  </si>
-  <si>
     <t>Event ERD</t>
   </si>
   <si>
     <t>Mikaeil and Ilia</t>
   </si>
   <si>
-    <t>03.03.</t>
-  </si>
-  <si>
     <t>Authenticator testing</t>
   </si>
   <si>
     <t>Process report</t>
   </si>
   <si>
-    <t>05.03.</t>
-  </si>
-  <si>
     <t>Initial application setup</t>
   </si>
   <si>
-    <t>10.03.</t>
-  </si>
-  <si>
     <t>Paypal converter for C#</t>
   </si>
   <si>
     <t>Research on future tech</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Date and hour started</t>
+  </si>
+  <si>
+    <t>06.03. || 15:00</t>
+  </si>
+  <si>
+    <t>11.03. || 18:48</t>
+  </si>
+  <si>
+    <t>10.03. || 20:00</t>
+  </si>
+  <si>
+    <t>25.02. || ?</t>
+  </si>
+  <si>
+    <t>26.02. || ?</t>
+  </si>
+  <si>
+    <t>23.02. || ?</t>
+  </si>
+  <si>
+    <t>03.03. || ?</t>
+  </si>
+  <si>
+    <t>07.03. || ?</t>
+  </si>
+  <si>
+    <t>9.03. || ?</t>
+  </si>
+  <si>
+    <t>05.03. || ?</t>
+  </si>
+  <si>
+    <t>21.02. || ?</t>
+  </si>
+  <si>
+    <t>21.02-02.03 || ?</t>
+  </si>
+  <si>
+    <t>10.03. || ?</t>
+  </si>
+  <si>
+    <t>as a Group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +160,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,8 +211,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -293,11 +335,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -353,9 +512,52 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -413,7 +615,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -448,7 +650,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -657,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +876,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -682,24 +884,33 @@
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>15</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D2" s="8">
         <v>120</v>
@@ -707,16 +918,27 @@
       <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="28">
+        <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
+        <v>60</v>
+      </c>
+      <c r="L2" s="29">
+        <f>ROUND((K2)/60,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5">
         <v>100</v>
@@ -724,191 +946,287 @@
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="J3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="21">
+        <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
+        <v>420</v>
+      </c>
+      <c r="L3" s="22">
+        <f t="shared" ref="L3:L7" si="0">ROUND((K3)/60,2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="5">
+        <v>100</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="J4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="21">
+        <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
+        <v>735</v>
+      </c>
+      <c r="L4" s="22">
+        <f t="shared" si="0"/>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="9">
+        <v>120</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="21">
+        <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
+        <v>160</v>
+      </c>
+      <c r="L5" s="22">
+        <f t="shared" si="0"/>
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="9">
+        <v>120</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="J6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="21">
+        <f>SUM(K2:K5)</f>
+        <v>1375</v>
+      </c>
+      <c r="L6" s="22">
+        <f t="shared" si="0"/>
+        <v>22.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="9">
+        <v>180</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="25">
+        <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*",B:B, "&lt;&gt;*"&amp;J5&amp;"*")</f>
+        <v>60</v>
+      </c>
+      <c r="L7" s="26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="5">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="9">
-        <v>480</v>
-      </c>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="5">
+    </row>
+    <row r="11" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="C11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="12" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="C12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="9">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="9">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="9">
-        <v>9.0299999999999994</v>
-      </c>
-      <c r="D10" s="9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="9">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>34</v>
+    <row r="13" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="10" t="s">
+    <row r="19" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="C19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="5">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -988,7 +1306,38 @@
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added to database example connection string for future use Rearanged tasks, added some time values V1 of AUTO Task coloring TODO for the formatting : https://exceljet.net/formula/cell-contains-specific-text
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$36</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Worked by:</t>
   </si>
@@ -37,15 +40,9 @@
     <t>Project plan v1</t>
   </si>
   <si>
-    <t>Google code</t>
-  </si>
-  <si>
     <t>Ilia</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>Base documents (agenda, notes and meeting)</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>Mikaeil and Ilia</t>
   </si>
   <si>
-    <t>Authenticator testing</t>
-  </si>
-  <si>
     <t>Process report</t>
   </si>
   <si>
@@ -115,43 +109,70 @@
     <t>10.03. || 20:00</t>
   </si>
   <si>
-    <t>25.02. || ?</t>
-  </si>
-  <si>
-    <t>26.02. || ?</t>
-  </si>
-  <si>
-    <t>23.02. || ?</t>
-  </si>
-  <si>
-    <t>03.03. || ?</t>
-  </si>
-  <si>
-    <t>07.03. || ?</t>
-  </si>
-  <si>
-    <t>9.03. || ?</t>
-  </si>
-  <si>
-    <t>05.03. || ?</t>
-  </si>
-  <si>
-    <t>21.02. || ?</t>
-  </si>
-  <si>
-    <t>21.02-02.03 || ?</t>
-  </si>
-  <si>
-    <t>10.03. || ?</t>
-  </si>
-  <si>
     <t>as a Group</t>
+  </si>
+  <si>
+    <t>Georgi and Ilia</t>
+  </si>
+  <si>
+    <t>Georgi and Ilia and Mikaeil</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>SVN:Google code</t>
+  </si>
+  <si>
+    <t>DOT research Framework</t>
+  </si>
+  <si>
+    <t>25.02. || 15:00</t>
+  </si>
+  <si>
+    <t>19.02. || 14:20</t>
+  </si>
+  <si>
+    <t>26.02. || 15:50</t>
+  </si>
+  <si>
+    <t>Phidgit Authenticator testing</t>
+  </si>
+  <si>
+    <t>9.03. || 10:40</t>
+  </si>
+  <si>
+    <t>10.03. || 19:00</t>
+  </si>
+  <si>
+    <t>02.03. || 16:45</t>
+  </si>
+  <si>
+    <t>21.02. || ??:??</t>
+  </si>
+  <si>
+    <t>23.02. || ??:??</t>
+  </si>
+  <si>
+    <t>05.03. || ??:??</t>
+  </si>
+  <si>
+    <t>07.03. || ??:??</t>
+  </si>
+  <si>
+    <t>10.03. || 23:20</t>
+  </si>
+  <si>
+    <t>11.03. || 22:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm\.dd\.\ \|\|\ hh:mm"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,8 +237,14 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -451,12 +478,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -552,6 +677,57 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -559,7 +735,57 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -859,67 +1085,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="47" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>29</v>
+      <c r="C1" s="42" t="s">
+        <v>26</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L1" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="8">
-        <v>120</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="5">
+        <v>100</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K2" s="28">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
@@ -929,414 +1157,480 @@
         <f>ROUND((K2)/60,2)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="5">
-        <v>100</v>
+      <c r="M2" s="22" t="str">
+        <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
+        <v>4%</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="8">
+        <v>120</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K3" s="21">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
         <v>420</v>
       </c>
       <c r="L3" s="22">
-        <f t="shared" ref="L3:L7" si="0">ROUND((K3)/60,2)</f>
+        <f t="shared" ref="L3:L5" si="0">ROUND((K3)/60,2)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="5">
-        <v>100</v>
+      <c r="M3" s="22" t="str">
+        <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
+        <v>28%</v>
+      </c>
+      <c r="O3" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="48">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
+        <v>60</v>
+      </c>
+      <c r="Q3" s="41">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="41">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="41">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="9">
+        <v>110</v>
       </c>
       <c r="H4" s="18"/>
       <c r="J4" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K4" s="21">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>735</v>
+        <v>760</v>
       </c>
       <c r="L4" s="22">
         <f t="shared" si="0"/>
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+        <v>12.67</v>
+      </c>
+      <c r="M4" s="22" t="str">
+        <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
+        <v>50%</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="48">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
+        <v>420</v>
+      </c>
+      <c r="R4" s="40">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
+        <v>220</v>
+      </c>
+      <c r="S4" s="40">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="5">
+        <v>60</v>
+      </c>
+      <c r="J5" s="23" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="9">
-        <v>120</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>15</v>
       </c>
       <c r="K5" s="21">
         <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
-        <v>160</v>
+        <v>280</v>
       </c>
       <c r="L5" s="22">
         <f t="shared" si="0"/>
-        <v>2.67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="9" t="s">
+        <v>4.67</v>
+      </c>
+      <c r="M5" s="22" t="str">
+        <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
+        <v>18%</v>
+      </c>
+      <c r="O5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="48">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
+        <v>760</v>
+      </c>
+      <c r="S5" s="40">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="J6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="9">
-        <v>120</v>
-      </c>
-      <c r="H6" s="20"/>
-      <c r="J6" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="21">
-        <f>SUM(K2:K5)</f>
-        <v>1375</v>
-      </c>
-      <c r="L6" s="22">
-        <f t="shared" si="0"/>
-        <v>22.92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="9">
-        <v>180</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="25">
+      <c r="K6" s="25">
         <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*",B:B, "&lt;&gt;*"&amp;J5&amp;"*")</f>
         <v>60</v>
       </c>
-      <c r="L7" s="26">
-        <f t="shared" si="0"/>
+      <c r="L6" s="26">
+        <f>ROUND((K6)/60,2)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="26" t="str">
+        <f>ROUND(($K$6) / ($K$7), 2) * 100 &amp;"%"</f>
+        <v>4%</v>
+      </c>
+      <c r="O6" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="49">
+        <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O6&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="5">
+        <v>65</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="21">
+        <f>SUM(K2:K5)</f>
+        <v>1520</v>
+      </c>
+      <c r="L7" s="22">
+        <f>ROUND((K7)/60,2)</f>
+        <v>25.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>27</v>
       </c>
       <c r="D8" s="9">
         <v>120</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="e">
+        <f>IF(A2=H9, A2:D2, FALSE)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="9">
+        <v>90</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="C10" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="C12" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="9">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+    <row r="14" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
+    </row>
+    <row r="15" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="9">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="9">
+      <c r="B15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="9">
-        <v>90</v>
-      </c>
-    </row>
     <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="5">
-        <v>60</v>
-      </c>
+      <c r="A17" s="6"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="5">
-        <v>10</v>
-      </c>
+      <c r="A18" s="6"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="5">
-        <v>60</v>
-      </c>
+      <c r="A19" s="6"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="12"/>
-      <c r="C21" s="6"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="6"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="12"/>
-      <c r="C23" s="6"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="6"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="6"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="6"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="6"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="6"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="12"/>
-      <c r="C29" s="6"/>
+      <c r="C29" s="46"/>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="6"/>
+      <c r="C30" s="46"/>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="6"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="12"/>
-      <c r="C32" s="6"/>
+      <c r="C32" s="46"/>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="12"/>
-      <c r="C33" s="6"/>
+      <c r="C33" s="46"/>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="12"/>
-      <c r="C34" s="6"/>
+      <c r="C34" s="46"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:D16">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>IF($A2 = $H9, IF($I9 &lt;&gt;  "Y", TRUE, FALSE), FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>IF($A1048571 = $H2, IF($I2 =  "Y", TRUE, FALSE), FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Test via Source Tree Removed auto color formatting
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Worked by:</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>Georgi and Ilia and Mikaeil</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>SVN:Google code</t>
@@ -171,7 +168,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm\.dd\.\ \|\|\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="mm\.dd\.\ \|\|\ hh:mm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -706,22 +703,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -735,14 +732,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -754,34 +744,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1088,7 +1050,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1100,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5">
         <v>100</v>
@@ -1182,7 +1144,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="8">
         <v>120</v>
@@ -1233,7 +1195,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="9">
         <v>110</v>
@@ -1273,13 +1235,13 @@
     </row>
     <row r="5" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="5">
         <v>60</v>
@@ -1315,13 +1277,13 @@
     </row>
     <row r="6" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
@@ -1355,13 +1317,13 @@
     </row>
     <row r="7" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="5">
         <v>65</v>
@@ -1391,10 +1353,6 @@
       <c r="D8" s="9">
         <v>120</v>
       </c>
-      <c r="G8" s="1" t="e">
-        <f>IF(A2=H9, A2:D2, FALSE)</f>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row r="9" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1404,16 +1362,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="9">
         <v>90</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1424,7 +1376,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="9">
         <v>60</v>
@@ -1438,7 +1390,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="9">
         <v>40</v>
@@ -1466,7 +1418,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="5">
         <v>60</v>
@@ -1480,7 +1432,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="5">
         <v>10</v>
@@ -1508,7 +1460,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="5">
         <v>60</v>
@@ -1623,14 +1575,6 @@
       <c r="D34" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:D16">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>IF($A2 = $H9, IF($I9 &lt;&gt;  "Y", TRUE, FALSE), FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>IF($A1048571 = $H2, IF($I2 =  "Y", TRUE, FALSE), FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Agenda for next week and tasks
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$38</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
   <si>
     <t>Worked by:</t>
   </si>
@@ -145,22 +145,64 @@
     <t>02.03. || 16:45</t>
   </si>
   <si>
-    <t>21.02. || ??:??</t>
-  </si>
-  <si>
-    <t>23.02. || ??:??</t>
-  </si>
-  <si>
-    <t>05.03. || ??:??</t>
-  </si>
-  <si>
-    <t>07.03. || ??:??</t>
-  </si>
-  <si>
     <t>10.03. || 23:20</t>
   </si>
   <si>
     <t>11.03. || 22:00</t>
+  </si>
+  <si>
+    <t>Database design and implementation</t>
+  </si>
+  <si>
+    <t>12.03. ||19:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphical design </t>
+  </si>
+  <si>
+    <t>12.03. || 20:00</t>
+  </si>
+  <si>
+    <t>User interface</t>
+  </si>
+  <si>
+    <t>12.03. || 20:30</t>
+  </si>
+  <si>
+    <t>Transfer to GITHub</t>
+  </si>
+  <si>
+    <t>14.03. || 02:10</t>
+  </si>
+  <si>
+    <t>23.02. || 15:30</t>
+  </si>
+  <si>
+    <t>21.02. || 19:10</t>
+  </si>
+  <si>
+    <t>05.03. || 18:10</t>
+  </si>
+  <si>
+    <t>07.03. || 14:20</t>
+  </si>
+  <si>
+    <t>05.03. || 17:20</t>
+  </si>
+  <si>
+    <t>12.03. || 16:10</t>
+  </si>
+  <si>
+    <t>14.03. || 02:40</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
   </si>
 </sst>
 </file>
@@ -241,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -335,19 +377,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -573,12 +602,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -625,106 +732,124 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -732,22 +857,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -803,7 +913,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -838,7 +948,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1047,19 +1157,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="47" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="44" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="5" max="5" width="14" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
@@ -1067,28 +1178,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="50" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="30" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1099,40 +1210,43 @@
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="41" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="5">
         <v>100</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="28">
+      <c r="K2" s="26">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
         <v>60</v>
       </c>
-      <c r="L2" s="29">
+      <c r="L2" s="27">
         <f>ROUND((K2)/60,2)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="22" t="str">
+      <c r="M2" s="20" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>4%</v>
+        <v>3%</v>
       </c>
       <c r="P2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="S2" s="16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1143,8 +1257,8 @@
       <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="43" t="s">
-        <v>42</v>
+      <c r="C3" s="40" t="s">
+        <v>53</v>
       </c>
       <c r="D3" s="8">
         <v>120</v>
@@ -1152,83 +1266,83 @@
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="19">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>420</v>
-      </c>
-      <c r="L3" s="22">
+        <v>480</v>
+      </c>
+      <c r="L3" s="20">
         <f t="shared" ref="L3:L5" si="0">ROUND((K3)/60,2)</f>
-        <v>7</v>
-      </c>
-      <c r="M3" s="22" t="str">
+        <v>8</v>
+      </c>
+      <c r="M3" s="20" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
         <v>28%</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="O3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="48">
+      <c r="P3" s="45">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
         <v>60</v>
       </c>
-      <c r="Q3" s="41">
+      <c r="Q3" s="39">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
         <v>0</v>
       </c>
-      <c r="R3" s="41">
+      <c r="R3" s="39">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
         <v>0</v>
       </c>
-      <c r="S3" s="41">
+      <c r="S3" s="39">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="9">
-        <v>110</v>
-      </c>
-      <c r="H4" s="18"/>
-      <c r="J4" s="23" t="s">
+      <c r="C4" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="5">
+        <v>60</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="J4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="19">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>760</v>
-      </c>
-      <c r="L4" s="22">
+        <v>765</v>
+      </c>
+      <c r="L4" s="20">
         <f t="shared" si="0"/>
-        <v>12.67</v>
-      </c>
-      <c r="M4" s="22" t="str">
+        <v>12.75</v>
+      </c>
+      <c r="M4" s="20" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>50%</v>
-      </c>
-      <c r="O4" s="34" t="s">
+        <v>45%</v>
+      </c>
+      <c r="O4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="48">
+      <c r="P4" s="31"/>
+      <c r="Q4" s="45">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>420</v>
-      </c>
-      <c r="R4" s="40">
+        <v>480</v>
+      </c>
+      <c r="R4" s="38">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
         <v>220</v>
       </c>
-      <c r="S4" s="40">
+      <c r="S4" s="38">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>120</v>
       </c>
@@ -1240,37 +1354,37 @@
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="41" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="5">
         <v>60</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="21">
+      <c r="K5" s="19">
         <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
-        <v>280</v>
-      </c>
-      <c r="L5" s="22">
+        <v>410</v>
+      </c>
+      <c r="L5" s="20">
         <f t="shared" si="0"/>
-        <v>4.67</v>
-      </c>
-      <c r="M5" s="22" t="str">
+        <v>6.83</v>
+      </c>
+      <c r="M5" s="20" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>18%</v>
-      </c>
-      <c r="O5" s="34" t="s">
+        <v>24%</v>
+      </c>
+      <c r="O5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="48">
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="45">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>760</v>
-      </c>
-      <c r="S5" s="40">
+        <v>765</v>
+      </c>
+      <c r="S5" s="38">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>160</v>
       </c>
@@ -1282,297 +1396,369 @@
       <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="41" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="J6" s="24" t="s">
+      <c r="H6" s="18"/>
+      <c r="J6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="23">
         <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*",B:B, "&lt;&gt;*"&amp;J5&amp;"*")</f>
         <v>60</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="24">
         <f>ROUND((K6)/60,2)</f>
         <v>1</v>
       </c>
-      <c r="M6" s="26" t="str">
+      <c r="M6" s="24" t="str">
         <f>ROUND(($K$6) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>4%</v>
-      </c>
-      <c r="O6" s="35" t="s">
+        <v>3%</v>
+      </c>
+      <c r="O6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="49">
+      <c r="P6" s="35"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="46">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O6&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
-        <v>280</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="55">
         <v>65</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="19">
         <f>SUM(K2:K5)</f>
-        <v>1520</v>
-      </c>
-      <c r="L7" s="22">
+        <v>1715</v>
+      </c>
+      <c r="L7" s="20">
         <f>ROUND((K7)/60,2)</f>
-        <v>25.33</v>
+        <v>28.58</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>120</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="9">
+      <c r="C10" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="5">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B11" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="C11" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="55">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="12" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C12" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D12" s="8">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="9">
-        <v>180</v>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="44" t="s">
-        <v>40</v>
+      <c r="C13" s="41" t="s">
+        <v>29</v>
       </c>
       <c r="D13" s="5">
-        <v>60</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="44" t="s">
-        <v>46</v>
+      <c r="C14" s="41" t="s">
+        <v>40</v>
       </c>
       <c r="D14" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="5">
         <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="9">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="5">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="6"/>
+      <c r="A21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="5">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="46"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="46"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="46"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="46"/>
+      <c r="C27" s="43"/>
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="46"/>
+      <c r="C28" s="43"/>
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="12"/>
-      <c r="C29" s="46"/>
+      <c r="C29" s="43"/>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="46"/>
+      <c r="C30" s="43"/>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="46"/>
+      <c r="C31" s="43"/>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="12"/>
-      <c r="C32" s="46"/>
+      <c r="C32" s="43"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="12"/>
-      <c r="C33" s="46"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="12"/>
-      <c r="C34" s="46"/>
+      <c r="C34" s="43"/>
       <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated agenda and tasks after meeting
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Worked by:</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>13.03. || 16:40</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Group meeting</t>
+  </si>
+  <si>
+    <t>Georgi, Mikaeil and Ilia</t>
+  </si>
+  <si>
+    <t>16.03. || 11:00</t>
   </si>
 </sst>
 </file>
@@ -694,7 +706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -860,15 +872,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1187,7 +1190,7 @@
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,15 +1301,15 @@
       </c>
       <c r="K3" s="17">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>541</v>
+        <v>574</v>
       </c>
       <c r="L3" s="18">
         <f t="shared" ref="L3:L5" si="0">ROUND((K3)/60,2)</f>
-        <v>9.02</v>
+        <v>9.57</v>
       </c>
       <c r="M3" s="18" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>29%</v>
+        <v>30%</v>
       </c>
       <c r="O3" s="32" t="s">
         <v>15</v>
@@ -1347,15 +1350,15 @@
       </c>
       <c r="K4" s="17">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>826</v>
+        <v>859</v>
       </c>
       <c r="L4" s="18">
         <f t="shared" si="0"/>
-        <v>13.77</v>
+        <v>14.32</v>
       </c>
       <c r="M4" s="18" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>45%</v>
+        <v>44%</v>
       </c>
       <c r="O4" s="30" t="s">
         <v>9</v>
@@ -1363,15 +1366,15 @@
       <c r="P4" s="29"/>
       <c r="Q4" s="42">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>541</v>
+        <v>574</v>
       </c>
       <c r="R4" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="S4" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
-        <v>120</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1392,15 +1395,15 @@
       </c>
       <c r="K5" s="17">
         <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
-        <v>410</v>
+        <v>443</v>
       </c>
       <c r="L5" s="18">
         <f t="shared" si="0"/>
-        <v>6.83</v>
+        <v>7.38</v>
       </c>
       <c r="M5" s="18" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>22%</v>
+        <v>23%</v>
       </c>
       <c r="O5" s="30" t="s">
         <v>7</v>
@@ -1409,11 +1412,11 @@
       <c r="Q5" s="29"/>
       <c r="R5" s="42">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>826</v>
+        <v>859</v>
       </c>
       <c r="S5" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
-        <v>160</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1453,7 +1456,7 @@
       <c r="R6" s="35"/>
       <c r="S6" s="43">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O6&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
-        <v>410</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1474,11 +1477,11 @@
       </c>
       <c r="K7" s="17">
         <f>SUM(K2:K5)</f>
-        <v>1837</v>
+        <v>1936</v>
       </c>
       <c r="L7" s="18">
         <f>ROUND((K7)/60,2)</f>
-        <v>30.62</v>
+        <v>32.270000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1613,7 +1616,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
@@ -1655,7 +1658,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>46</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>48</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="55" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="55" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
@@ -1697,7 +1700,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
@@ -1711,61 +1714,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="59" t="s">
+    <row r="24" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="59"/>
-    </row>
-    <row r="25" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="56"/>
-    </row>
-    <row r="26" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="56"/>
+    </row>
+    <row r="25" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="8">
+        <v>33</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="10"/>
       <c r="C26" s="40"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="10"/>
       <c r="C27" s="40"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="10"/>
       <c r="C28" s="40"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="10"/>
       <c r="C29" s="40"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="10"/>
       <c r="C30" s="40"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="10"/>
       <c r="C31" s="40"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="10"/>
       <c r="C32" s="40"/>

</xml_diff>

<commit_message>
Setup document draft 1 and part of the tasks for the week
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>Worked by:</t>
   </si>
@@ -224,6 +224,15 @@
   </si>
   <si>
     <t>16.03. || 11:00</t>
+  </si>
+  <si>
+    <t>17.03. || 16:00</t>
+  </si>
+  <si>
+    <t>21.03. || 17:00</t>
+  </si>
+  <si>
+    <t>Setup document v1</t>
   </si>
 </sst>
 </file>
@@ -1189,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,15 +1310,15 @@
       </c>
       <c r="K3" s="17">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>574</v>
+        <v>734</v>
       </c>
       <c r="L3" s="18">
         <f t="shared" ref="L3:L5" si="0">ROUND((K3)/60,2)</f>
-        <v>9.57</v>
+        <v>12.23</v>
       </c>
       <c r="M3" s="18" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>30%</v>
+        <v>33%</v>
       </c>
       <c r="O3" s="32" t="s">
         <v>15</v>
@@ -1350,11 +1359,11 @@
       </c>
       <c r="K4" s="17">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>859</v>
+        <v>979</v>
       </c>
       <c r="L4" s="18">
         <f t="shared" si="0"/>
-        <v>14.32</v>
+        <v>16.32</v>
       </c>
       <c r="M4" s="18" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
@@ -1366,11 +1375,11 @@
       <c r="P4" s="29"/>
       <c r="Q4" s="42">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>574</v>
+        <v>734</v>
       </c>
       <c r="R4" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>314</v>
+        <v>434</v>
       </c>
       <c r="S4" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1403,7 +1412,7 @@
       </c>
       <c r="M5" s="18" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>23%</v>
+        <v>20%</v>
       </c>
       <c r="O5" s="30" t="s">
         <v>7</v>
@@ -1412,7 +1421,7 @@
       <c r="Q5" s="29"/>
       <c r="R5" s="42">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>859</v>
+        <v>979</v>
       </c>
       <c r="S5" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1477,11 +1486,11 @@
       </c>
       <c r="K7" s="17">
         <f>SUM(K2:K5)</f>
-        <v>1936</v>
+        <v>2216</v>
       </c>
       <c r="L7" s="18">
         <f>ROUND((K7)/60,2)</f>
-        <v>32.270000000000003</v>
+        <v>36.93</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1744,16 +1753,32 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="6"/>
+      <c r="A26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="5">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="5">
+        <v>120</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>

</xml_diff>

<commit_message>
Updated main documentation and fixed 2 problems on Setup doc
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$42</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
   <si>
     <t>Worked by:</t>
   </si>
@@ -233,6 +233,42 @@
   </si>
   <si>
     <t>Setup document v1</t>
+  </si>
+  <si>
+    <t>23.03. || 11:00</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Websitedesign</t>
+  </si>
+  <si>
+    <t>09.03. || 16:00</t>
+  </si>
+  <si>
+    <t>Wireframe</t>
+  </si>
+  <si>
+    <t>21.03. || 15:30</t>
+  </si>
+  <si>
+    <t>Website design</t>
+  </si>
+  <si>
+    <t>21.03. || 16:30</t>
+  </si>
+  <si>
+    <t>Application GUI</t>
+  </si>
+  <si>
+    <t>Setup document v2</t>
+  </si>
+  <si>
+    <t>23.03. || 10:30</t>
+  </si>
+  <si>
+    <t>23.03. || 11:10</t>
   </si>
 </sst>
 </file>
@@ -313,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -708,6 +744,30 @@
       <bottom style="mediumDashed">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -715,7 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -889,6 +949,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1196,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,15 +1338,15 @@
       </c>
       <c r="K2" s="24">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="L2" s="25">
         <f>ROUND((K2)/60,2)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M2" s="18" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>3%</v>
+        <v>10%</v>
       </c>
       <c r="P2" s="12" t="s">
         <v>15</v>
@@ -1310,22 +1382,22 @@
       </c>
       <c r="K3" s="17">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>734</v>
+        <v>894</v>
       </c>
       <c r="L3" s="18">
         <f t="shared" ref="L3:L5" si="0">ROUND((K3)/60,2)</f>
-        <v>12.23</v>
+        <v>14.9</v>
       </c>
       <c r="M3" s="18" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>33%</v>
+        <v>31%</v>
       </c>
       <c r="O3" s="32" t="s">
         <v>15</v>
       </c>
       <c r="P3" s="42">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="Q3" s="37">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
@@ -1359,15 +1431,15 @@
       </c>
       <c r="K4" s="17">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>979</v>
+        <v>1119</v>
       </c>
       <c r="L4" s="18">
         <f t="shared" si="0"/>
-        <v>16.32</v>
+        <v>18.649999999999999</v>
       </c>
       <c r="M4" s="18" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>44%</v>
+        <v>39%</v>
       </c>
       <c r="O4" s="30" t="s">
         <v>9</v>
@@ -1375,7 +1447,7 @@
       <c r="P4" s="29"/>
       <c r="Q4" s="42">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>734</v>
+        <v>894</v>
       </c>
       <c r="R4" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
@@ -1404,11 +1476,11 @@
       </c>
       <c r="K5" s="17">
         <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
-        <v>443</v>
+        <v>583</v>
       </c>
       <c r="L5" s="18">
         <f t="shared" si="0"/>
-        <v>7.38</v>
+        <v>9.7200000000000006</v>
       </c>
       <c r="M5" s="18" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
@@ -1421,11 +1493,11 @@
       <c r="Q5" s="29"/>
       <c r="R5" s="42">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>979</v>
+        <v>1119</v>
       </c>
       <c r="S5" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
-        <v>193</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,11 +1519,11 @@
       </c>
       <c r="K6" s="21">
         <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*",B:B, "&lt;&gt;*"&amp;J5&amp;"*")</f>
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="L6" s="22">
         <f>ROUND((K6)/60,2)</f>
-        <v>1</v>
+        <v>1.67</v>
       </c>
       <c r="M6" s="22" t="str">
         <f>ROUND(($K$6) / ($K$7), 2) * 100 &amp;"%"</f>
@@ -1465,7 +1537,7 @@
       <c r="R6" s="35"/>
       <c r="S6" s="43">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O6&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
-        <v>443</v>
+        <v>583</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1486,11 +1558,11 @@
       </c>
       <c r="K7" s="17">
         <f>SUM(K2:K5)</f>
-        <v>2216</v>
+        <v>2896</v>
       </c>
       <c r="L7" s="18">
         <f>ROUND((K7)/60,2)</f>
-        <v>36.93</v>
+        <v>48.27</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1570,84 +1642,84 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="5">
-        <v>180</v>
+      <c r="A13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="8">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D14" s="5">
-        <v>60</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" s="5">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D16" s="5">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="39" t="s">
         <v>43</v>
-      </c>
-      <c r="D17" s="5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>57</v>
       </c>
       <c r="D18" s="5">
         <v>60</v>
@@ -1655,172 +1727,231 @@
     </row>
     <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D19" s="5">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>46</v>
+      <c r="A20" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D20" s="5">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D22" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="55" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="23" spans="1:5" s="55" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B23" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C23" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D23" s="7">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C24" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D24" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="56" t="s">
+    <row r="25" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="57" t="s">
+      <c r="B25" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="58" t="s">
+      <c r="C25" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="56"/>
-    </row>
-    <row r="25" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="D25" s="56"/>
+    </row>
+    <row r="26" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C26" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D26" s="8">
         <v>33</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="27" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C27" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D27" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B30" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C30" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D30" s="52">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="6"/>
-    </row>
     <row r="31" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="8">
+        <v>40</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="6"/>
+      <c r="A32" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="5">
+        <v>60</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="6"/>
+      <c r="A33" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="5">
+        <v>140</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="6"/>
+      <c r="A34" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="5">
+        <v>100</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
@@ -1828,17 +1959,35 @@
       <c r="C35" s="40"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="10"/>
       <c r="C36" s="40"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="10"/>
       <c r="C37" s="40"/>
       <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated agenda and tasks for previous days
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$46</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t>Worked by:</t>
   </si>
@@ -266,6 +266,45 @@
   </si>
   <si>
     <t>23.03. || 11:10</t>
+  </si>
+  <si>
+    <t>Website frontpage</t>
+  </si>
+  <si>
+    <t>25.03. || 16:00</t>
+  </si>
+  <si>
+    <t>Website wireframe</t>
+  </si>
+  <si>
+    <t>23.03. || 13:20</t>
+  </si>
+  <si>
+    <t>GUI design</t>
+  </si>
+  <si>
+    <t>23.03. || 09:00</t>
+  </si>
+  <si>
+    <t>25.03. || 20:00</t>
+  </si>
+  <si>
+    <t>Database review</t>
+  </si>
+  <si>
+    <t>25.03. || 22:00</t>
+  </si>
+  <si>
+    <t>Website review</t>
+  </si>
+  <si>
+    <t>Angel and Georgi</t>
+  </si>
+  <si>
+    <t>26.03. || 12:00</t>
+  </si>
+  <si>
+    <t>24.03. || 13:00</t>
   </si>
 </sst>
 </file>
@@ -1015,6 +1054,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1062,7 +1104,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1097,7 +1139,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1306,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,15 +1418,15 @@
       </c>
       <c r="K2" s="24">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
-        <v>180</v>
+        <v>460</v>
       </c>
       <c r="L2" s="76" t="str">
         <f t="shared" ref="L2:L5" si="0">ROUNDDOWN((K2)/60,0) &amp;":"&amp;(IF(MOD(K2, 60) &lt; 10, "0","")) &amp; MOD(K2,60)</f>
-        <v>3:00</v>
+        <v>7:40</v>
       </c>
       <c r="M2" s="18" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>6%</v>
+        <v>12%</v>
       </c>
       <c r="P2" s="12" t="s">
         <v>15</v>
@@ -1420,26 +1462,26 @@
       </c>
       <c r="K3" s="17">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>941</v>
+        <v>981</v>
       </c>
       <c r="L3" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>15:41</v>
+        <v>16:21</v>
       </c>
       <c r="M3" s="18" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>32%</v>
+        <v>25%</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>15</v>
       </c>
       <c r="P3" s="41">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
-        <v>180</v>
+        <v>460</v>
       </c>
       <c r="Q3" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R3" s="36">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
@@ -1469,15 +1511,15 @@
       </c>
       <c r="K4" s="17">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>1166</v>
+        <v>1436</v>
       </c>
       <c r="L4" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>19:26</v>
+        <v>23:56</v>
       </c>
       <c r="M4" s="18" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>40%</v>
+        <v>37%</v>
       </c>
       <c r="O4" s="29" t="s">
         <v>9</v>
@@ -1485,7 +1527,7 @@
       <c r="P4" s="28"/>
       <c r="Q4" s="41">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>941</v>
+        <v>981</v>
       </c>
       <c r="R4" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
@@ -1514,15 +1556,15 @@
       </c>
       <c r="K5" s="17">
         <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
-        <v>630</v>
+        <v>990</v>
       </c>
       <c r="L5" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>10:30</v>
+        <v>16:30</v>
       </c>
       <c r="M5" s="18" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>22%</v>
+        <v>26%</v>
       </c>
       <c r="O5" s="29" t="s">
         <v>7</v>
@@ -1531,7 +1573,7 @@
       <c r="Q5" s="28"/>
       <c r="R5" s="41">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>1166</v>
+        <v>1436</v>
       </c>
       <c r="S5" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1575,7 +1617,7 @@
       <c r="R6" s="34"/>
       <c r="S6" s="42">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O6&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
-        <v>630</v>
+        <v>990</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1596,11 +1638,11 @@
       </c>
       <c r="K7" s="17">
         <f>SUM(K2:K5)</f>
-        <v>2917</v>
+        <v>3867</v>
       </c>
       <c r="L7" s="76" t="str">
         <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
-        <v>48:37</v>
+        <v>64:27</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1904,112 +1946,226 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="67" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="65">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B30" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C30" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D30" s="65">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="78" t="s">
+    <row r="31" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="78" t="s">
+      <c r="B31" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="77" t="s">
+      <c r="C31" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="78">
+      <c r="D31" s="78">
         <v>120</v>
       </c>
-      <c r="E30" s="75"/>
-    </row>
-    <row r="31" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="70" t="s">
+      <c r="E31" s="75"/>
+    </row>
+    <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="72" t="s">
+      <c r="B32" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="73" t="s">
+      <c r="C32" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="70">
+      <c r="D32" s="70">
         <v>40</v>
       </c>
-      <c r="E31" s="67" t="s">
+      <c r="E32" s="67" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="69" t="s">
+    <row r="33" spans="1:5" s="67" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="73" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="70">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="69" t="s">
         <v>8</v>
-      </c>
-      <c r="B32" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="74" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="68">
-        <v>60</v>
-      </c>
-      <c r="E32" s="66"/>
-    </row>
-    <row r="33" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="74" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="68">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="68" t="s">
-        <v>81</v>
       </c>
       <c r="B34" s="71" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="74" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="68">
+        <v>60</v>
+      </c>
+      <c r="E34" s="66"/>
+    </row>
+    <row r="35" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="68">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="68">
+      <c r="D36" s="68">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="6"/>
+    <row r="37" spans="1:5" s="67" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="74" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="68">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="67" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="68">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="67" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="71" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" s="68">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="67" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="68">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="67" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="68">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="74" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="68">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="67" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="68">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Group by member total group work
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$47</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="113">
   <si>
     <t>Worked by:</t>
   </si>
@@ -436,7 +436,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -719,18 +719,135 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -739,122 +856,20 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="mediumDashed">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -862,7 +877,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -954,15 +969,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -981,37 +987,37 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1035,16 +1041,16 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1076,10 +1082,25 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1143,7 +1164,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1178,7 +1199,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1389,15 +1410,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="39" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="36" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
@@ -1408,16 +1429,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -1440,7 +1461,7 @@
       <c r="B2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="34" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="5">
@@ -1459,7 +1480,7 @@
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
         <v>730</v>
       </c>
-      <c r="L2" s="72" t="str">
+      <c r="L2" s="69" t="str">
         <f t="shared" ref="L2:L5" si="0">ROUNDDOWN((K2)/60,0) &amp;":"&amp;(IF(MOD(K2, 60) &lt; 10, "0","")) &amp; MOD(K2,60)</f>
         <v>12:10</v>
       </c>
@@ -1487,7 +1508,7 @@
       <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="33" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="8">
@@ -1503,7 +1524,7 @@
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
         <v>1351</v>
       </c>
-      <c r="L3" s="72" t="str">
+      <c r="L3" s="69" t="str">
         <f t="shared" si="0"/>
         <v>22:31</v>
       </c>
@@ -1514,19 +1535,19 @@
       <c r="O3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="40">
+      <c r="P3" s="37">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
         <v>730</v>
       </c>
-      <c r="Q3" s="35">
+      <c r="Q3" s="32">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
         <v>40</v>
       </c>
-      <c r="R3" s="35">
+      <c r="R3" s="32">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
         <v>0</v>
       </c>
-      <c r="S3" s="35">
+      <c r="S3" s="32">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>0</v>
       </c>
@@ -1538,7 +1559,7 @@
       <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="34" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="5">
@@ -1552,7 +1573,7 @@
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
         <v>1996</v>
       </c>
-      <c r="L4" s="72" t="str">
+      <c r="L4" s="69" t="str">
         <f t="shared" si="0"/>
         <v>33:16</v>
       </c>
@@ -1564,15 +1585,15 @@
         <v>9</v>
       </c>
       <c r="P4" s="27"/>
-      <c r="Q4" s="40">
+      <c r="Q4" s="37">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
         <v>1351</v>
       </c>
-      <c r="R4" s="34">
+      <c r="R4" s="31">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
         <v>601</v>
       </c>
-      <c r="S4" s="34">
+      <c r="S4" s="31">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>200</v>
       </c>
@@ -1584,7 +1605,7 @@
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="34" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="5">
@@ -1597,7 +1618,7 @@
         <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
         <v>990</v>
       </c>
-      <c r="L5" s="72" t="str">
+      <c r="L5" s="69" t="str">
         <f t="shared" si="0"/>
         <v>16:30</v>
       </c>
@@ -1610,11 +1631,11 @@
       </c>
       <c r="P5" s="27"/>
       <c r="Q5" s="27"/>
-      <c r="R5" s="40">
+      <c r="R5" s="37">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
         <v>1996</v>
       </c>
-      <c r="S5" s="34">
+      <c r="S5" s="31">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>380</v>
       </c>
@@ -1626,7 +1647,7 @@
       <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="34" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="5">
@@ -1640,7 +1661,7 @@
         <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*",B:B, "&lt;&gt;*"&amp;J5&amp;"*")</f>
         <v>100</v>
       </c>
-      <c r="L6" s="72" t="str">
+      <c r="L6" s="69" t="str">
         <f>ROUNDDOWN((K6)/60,0) &amp;":"&amp;(IF(MOD(K6, 60) &lt; 10, "0","")) &amp; MOD(K6,60)</f>
         <v>1:40</v>
       </c>
@@ -1651,25 +1672,25 @@
       <c r="O6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="41">
+      <c r="P6" s="73"/>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="75"/>
+      <c r="S6" s="38">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O6&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>990</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="47">
         <v>65</v>
       </c>
       <c r="J7" s="18" t="s">
@@ -1679,19 +1700,38 @@
         <f>SUM(K2:K5)</f>
         <v>5067</v>
       </c>
-      <c r="L7" s="72" t="str">
+      <c r="L7" s="69" t="str">
         <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
         <v>84:27</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="O7" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="76">
+        <f>Q3+R3+S3</f>
+        <v>40</v>
+      </c>
+      <c r="Q7" s="76">
+        <f>Q3+R4+S4</f>
+        <v>841</v>
+      </c>
+      <c r="R7" s="72">
+        <f>R3+R4+S5</f>
+        <v>981</v>
+      </c>
+      <c r="S7" s="72">
+        <f>S3+S4+S5</f>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="33" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="8">
@@ -1700,15 +1740,34 @@
       <c r="E8" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O8" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="76" t="str">
+        <f>ROUNDDOWN((P7)/60,0) &amp;":"&amp;(IF(MOD(P7, 60) &lt; 10, "0","")) &amp; MOD(P7,60)</f>
+        <v>0:40</v>
+      </c>
+      <c r="Q8" s="76" t="str">
+        <f t="shared" ref="Q8:S8" si="1">ROUNDDOWN((Q7)/60,0) &amp;":"&amp;(IF(MOD(Q7, 60) &lt; 10, "0","")) &amp; MOD(Q7,60)</f>
+        <v>14:01</v>
+      </c>
+      <c r="R8" s="76" t="str">
+        <f t="shared" si="1"/>
+        <v>16:21</v>
+      </c>
+      <c r="S8" s="72" t="str">
+        <f t="shared" si="1"/>
+        <v>9:40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="34" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="5">
@@ -1722,7 +1781,7 @@
       <c r="B10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="33" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="8">
@@ -1730,16 +1789,16 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="47">
         <v>60</v>
       </c>
     </row>
@@ -1750,7 +1809,7 @@
       <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="33" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="8">
@@ -1767,164 +1826,164 @@
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="34" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="5">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="34" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="34" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="34" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="5">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="34" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="34" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="34" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="34" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="53" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="50" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="49" t="s">
         <v>64</v>
       </c>
       <c r="D22" s="7">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="34" t="s">
         <v>51</v>
       </c>
       <c r="D23" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="74" t="s">
+    <row r="24" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="74">
+      <c r="D24" s="71">
         <v>60</v>
       </c>
     </row>
@@ -1935,7 +1994,7 @@
       <c r="B25" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="33" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="8">
@@ -1946,16 +2005,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="54">
+      <c r="D26" s="51">
         <v>40</v>
       </c>
     </row>
@@ -1966,7 +2025,7 @@
       <c r="B27" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="33" t="s">
         <v>72</v>
       </c>
       <c r="D27" s="8">
@@ -1974,287 +2033,287 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="60" t="s">
+      <c r="C28" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="61">
+      <c r="D28" s="58">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="58" t="s">
+    <row r="29" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="61">
+      <c r="D29" s="58">
         <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="59" t="s">
+      <c r="B30" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="60" t="s">
+      <c r="C30" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="61">
+      <c r="D30" s="58">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="73" t="s">
+      <c r="C31" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="74">
+      <c r="D31" s="71">
         <v>120</v>
       </c>
-      <c r="E31" s="71"/>
+      <c r="E31" s="68"/>
     </row>
     <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="69" t="s">
+      <c r="C32" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="66">
+      <c r="D32" s="63">
         <v>40</v>
       </c>
-      <c r="E32" s="63" t="s">
+      <c r="E32" s="60" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46" t="s">
+    <row r="33" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="69" t="s">
+      <c r="C33" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="66">
+      <c r="D33" s="63">
         <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="67" t="s">
+      <c r="B34" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="70" t="s">
+      <c r="C34" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="64">
+      <c r="D34" s="61">
         <v>120</v>
       </c>
-      <c r="E34" s="62"/>
+      <c r="E34" s="59"/>
     </row>
     <row r="35" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="67" t="s">
+      <c r="B35" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="70" t="s">
+      <c r="C35" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="64">
+      <c r="D35" s="61">
         <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="64" t="s">
+      <c r="A36" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="67" t="s">
+      <c r="B36" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="70" t="s">
+      <c r="C36" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="64">
+      <c r="D36" s="61">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="64" t="s">
+    <row r="37" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="67" t="s">
+      <c r="B37" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="70" t="s">
+      <c r="C37" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="64">
+      <c r="D37" s="61">
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="64" t="s">
+    <row r="38" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="67" t="s">
+      <c r="B38" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="70" t="s">
+      <c r="C38" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="64">
+      <c r="D38" s="61">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="65" t="s">
+    <row r="39" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="67" t="s">
+      <c r="B39" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="70" t="s">
+      <c r="C39" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="64">
+      <c r="D39" s="61">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="64" t="s">
+    <row r="40" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="67" t="s">
+      <c r="B40" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="70" t="s">
+      <c r="C40" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="64">
+      <c r="D40" s="61">
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="64" t="s">
+    <row r="41" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="67" t="s">
+      <c r="B41" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="70" t="s">
+      <c r="C41" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="64">
+      <c r="D41" s="61">
         <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="64" t="s">
+      <c r="A42" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="67" t="s">
+      <c r="B42" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="70" t="s">
+      <c r="C42" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="64">
+      <c r="D42" s="61">
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="64" t="s">
+    <row r="43" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="67" t="s">
+      <c r="B43" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="64">
+      <c r="D43" s="61">
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="64" t="s">
+      <c r="A44" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="64" t="s">
+      <c r="B44" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="70" t="s">
+      <c r="C44" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="64">
+      <c r="D44" s="61">
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="64" t="s">
+    <row r="45" spans="1:5" s="60" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="B45" s="64" t="s">
+      <c r="B45" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="D45" s="64">
+      <c r="D45" s="61">
         <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="74" t="s">
+      <c r="A46" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="74" t="s">
+      <c r="B46" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="73" t="s">
+      <c r="C46" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="74">
+      <c r="D46" s="71">
         <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="66" t="s">
+      <c r="B47" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="69" t="s">
+      <c r="C47" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="D47" s="66">
+      <c r="D47" s="63">
         <v>60</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -2262,72 +2321,72 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="64" t="s">
+      <c r="A48" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="64" t="s">
+      <c r="B48" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="70" t="s">
+      <c r="C48" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="64">
+      <c r="D48" s="61">
         <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="64" t="s">
+      <c r="A49" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="B49" s="64" t="s">
+      <c r="B49" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="70" t="s">
+      <c r="C49" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="64">
+      <c r="D49" s="61">
         <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="46" t="s">
+      <c r="A50" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="68" t="s">
+      <c r="B50" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="69" t="s">
+      <c r="C50" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="D50" s="66">
+      <c r="D50" s="63">
         <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="74" t="s">
+      <c r="A51" s="71" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="74" t="s">
+      <c r="B51" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="73" t="s">
+      <c r="C51" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="74">
+      <c r="D51" s="71">
         <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="66" t="s">
+      <c r="B52" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="69" t="s">
+      <c r="C52" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="D52" s="66">
+      <c r="D52" s="63">
         <v>60</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -2335,263 +2394,263 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="46" t="s">
+      <c r="A53" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="68" t="s">
+      <c r="B53" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="69" t="s">
+      <c r="C53" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="66">
+      <c r="D53" s="63">
         <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="38"/>
+      <c r="C54" s="35"/>
       <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="38"/>
+      <c r="C55" s="35"/>
       <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="38"/>
+      <c r="C56" s="35"/>
       <c r="D56" s="6"/>
     </row>
     <row r="57" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="38"/>
+      <c r="C57" s="35"/>
       <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="38"/>
+      <c r="C58" s="35"/>
       <c r="D58" s="6"/>
     </row>
     <row r="59" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="38"/>
+      <c r="C59" s="35"/>
       <c r="D59" s="6"/>
     </row>
     <row r="60" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="38"/>
+      <c r="C60" s="35"/>
       <c r="D60" s="6"/>
     </row>
     <row r="61" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="38"/>
+      <c r="C61" s="35"/>
       <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="38"/>
+      <c r="C62" s="35"/>
       <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="38"/>
+      <c r="C63" s="35"/>
       <c r="D63" s="6"/>
     </row>
     <row r="64" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="38"/>
+      <c r="C64" s="35"/>
       <c r="D64" s="6"/>
     </row>
     <row r="65" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="38"/>
+      <c r="C65" s="35"/>
       <c r="D65" s="6"/>
     </row>
     <row r="66" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="38"/>
+      <c r="C66" s="35"/>
       <c r="D66" s="6"/>
     </row>
     <row r="67" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="38"/>
+      <c r="C67" s="35"/>
       <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="38"/>
+      <c r="C68" s="35"/>
       <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="38"/>
+      <c r="C69" s="35"/>
       <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="38"/>
+      <c r="C70" s="35"/>
       <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="38"/>
+      <c r="C71" s="35"/>
       <c r="D71" s="6"/>
     </row>
     <row r="72" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="38"/>
+      <c r="C72" s="35"/>
       <c r="D72" s="6"/>
     </row>
     <row r="73" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="38"/>
+      <c r="C73" s="35"/>
       <c r="D73" s="6"/>
     </row>
     <row r="74" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="38"/>
+      <c r="C74" s="35"/>
       <c r="D74" s="6"/>
     </row>
     <row r="75" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="38"/>
+      <c r="C75" s="35"/>
       <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
-      <c r="C76" s="38"/>
+      <c r="C76" s="35"/>
       <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="38"/>
+      <c r="C77" s="35"/>
       <c r="D77" s="6"/>
     </row>
     <row r="78" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="38"/>
+      <c r="C78" s="35"/>
       <c r="D78" s="6"/>
     </row>
     <row r="79" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="38"/>
+      <c r="C79" s="35"/>
       <c r="D79" s="6"/>
     </row>
     <row r="80" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="38"/>
+      <c r="C80" s="35"/>
       <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
-      <c r="C81" s="38"/>
+      <c r="C81" s="35"/>
       <c r="D81" s="6"/>
     </row>
     <row r="82" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
-      <c r="C82" s="38"/>
+      <c r="C82" s="35"/>
       <c r="D82" s="6"/>
     </row>
     <row r="83" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
-      <c r="C83" s="38"/>
+      <c r="C83" s="35"/>
       <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
-      <c r="C84" s="38"/>
+      <c r="C84" s="35"/>
       <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
-      <c r="C85" s="38"/>
+      <c r="C85" s="35"/>
       <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
-      <c r="C86" s="38"/>
+      <c r="C86" s="35"/>
       <c r="D86" s="6"/>
     </row>
     <row r="87" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
-      <c r="C87" s="38"/>
+      <c r="C87" s="35"/>
       <c r="D87" s="6"/>
     </row>
     <row r="88" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
-      <c r="C88" s="38"/>
+      <c r="C88" s="35"/>
       <c r="D88" s="6"/>
     </row>
     <row r="89" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
-      <c r="C89" s="38"/>
+      <c r="C89" s="35"/>
       <c r="D89" s="6"/>
     </row>
     <row r="90" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
-      <c r="C90" s="38"/>
+      <c r="C90" s="35"/>
       <c r="D90" s="6"/>
     </row>
     <row r="91" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
-      <c r="C91" s="38"/>
+      <c r="C91" s="35"/>
       <c r="D91" s="6"/>
     </row>
     <row r="92" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
-      <c r="C92" s="38"/>
+      <c r="C92" s="35"/>
       <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
-      <c r="C93" s="38"/>
+      <c r="C93" s="35"/>
       <c r="D93" s="6"/>
     </row>
     <row r="94" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
-      <c r="C94" s="38"/>
+      <c r="C94" s="35"/>
       <c r="D94" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tasks and parts of setup doc and process rep
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$47</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="127">
   <si>
     <t>Worked by:</t>
   </si>
@@ -356,6 +356,48 @@
   </si>
   <si>
     <t>12.04. || 08:30</t>
+  </si>
+  <si>
+    <t>Map feature</t>
+  </si>
+  <si>
+    <t>Map zoom</t>
+  </si>
+  <si>
+    <t>Map translation</t>
+  </si>
+  <si>
+    <t>16.04. || 8:30</t>
+  </si>
+  <si>
+    <t>16.04. || 11:30</t>
+  </si>
+  <si>
+    <t>17.04. || 01:30</t>
+  </si>
+  <si>
+    <t>Map search function</t>
+  </si>
+  <si>
+    <t>18.04. || 04:30</t>
+  </si>
+  <si>
+    <t>17.04. || 12:00</t>
+  </si>
+  <si>
+    <t>18.04. || 13:00</t>
+  </si>
+  <si>
+    <t>Menu Inheritance</t>
+  </si>
+  <si>
+    <t>19.04. || 10:30</t>
+  </si>
+  <si>
+    <t>15.04. || 12:00</t>
+  </si>
+  <si>
+    <t>19.04. || 12:00</t>
   </si>
 </sst>
 </file>
@@ -436,7 +478,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -719,6 +761,37 @@
       </left>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -824,52 +897,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -877,7 +904,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -969,6 +996,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -987,37 +1023,37 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1041,16 +1077,16 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1082,25 +1118,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1164,7 +1185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1199,7 +1220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1408,17 +1429,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S94"/>
+  <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="39" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
@@ -1429,16 +1450,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="45" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -1461,7 +1482,7 @@
       <c r="B2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="37" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="5">
@@ -1478,15 +1499,15 @@
       </c>
       <c r="K2" s="23">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
-        <v>730</v>
-      </c>
-      <c r="L2" s="69" t="str">
+        <v>1090</v>
+      </c>
+      <c r="L2" s="72" t="str">
         <f t="shared" ref="L2:L5" si="0">ROUNDDOWN((K2)/60,0) &amp;":"&amp;(IF(MOD(K2, 60) &lt; 10, "0","")) &amp; MOD(K2,60)</f>
-        <v>12:10</v>
+        <v>18:10</v>
       </c>
       <c r="M2" s="17" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>14%</v>
+        <v>18%</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>15</v>
@@ -1508,7 +1529,7 @@
       <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="36" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="8">
@@ -1522,32 +1543,32 @@
       </c>
       <c r="K3" s="16">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>1351</v>
-      </c>
-      <c r="L3" s="69" t="str">
+        <v>1591</v>
+      </c>
+      <c r="L3" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>22:31</v>
+        <v>26:31</v>
       </c>
       <c r="M3" s="17" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>27%</v>
+        <v>26%</v>
       </c>
       <c r="O3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="37">
+      <c r="P3" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
-        <v>730</v>
-      </c>
-      <c r="Q3" s="32">
+        <v>1090</v>
+      </c>
+      <c r="Q3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
         <v>40</v>
       </c>
-      <c r="R3" s="32">
+      <c r="R3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
         <v>0</v>
       </c>
-      <c r="S3" s="32">
+      <c r="S3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>0</v>
       </c>
@@ -1559,7 +1580,7 @@
       <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="37" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="5">
@@ -1571,29 +1592,29 @@
       </c>
       <c r="K4" s="16">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>1996</v>
-      </c>
-      <c r="L4" s="69" t="str">
+        <v>2416</v>
+      </c>
+      <c r="L4" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>33:16</v>
+        <v>40:16</v>
       </c>
       <c r="M4" s="17" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>39%</v>
+        <v>40%</v>
       </c>
       <c r="O4" s="28" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="27"/>
-      <c r="Q4" s="37">
+      <c r="Q4" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>1351</v>
-      </c>
-      <c r="R4" s="31">
+        <v>1591</v>
+      </c>
+      <c r="R4" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
         <v>601</v>
       </c>
-      <c r="S4" s="31">
+      <c r="S4" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>200</v>
       </c>
@@ -1605,7 +1626,7 @@
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="37" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="5">
@@ -1618,24 +1639,24 @@
         <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
         <v>990</v>
       </c>
-      <c r="L5" s="69" t="str">
+      <c r="L5" s="72" t="str">
         <f t="shared" si="0"/>
         <v>16:30</v>
       </c>
       <c r="M5" s="17" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>20%</v>
+        <v>16%</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>7</v>
       </c>
       <c r="P5" s="27"/>
       <c r="Q5" s="27"/>
-      <c r="R5" s="37">
+      <c r="R5" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>1996</v>
-      </c>
-      <c r="S5" s="31">
+        <v>2416</v>
+      </c>
+      <c r="S5" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>380</v>
       </c>
@@ -1647,7 +1668,7 @@
       <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="37" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="5">
@@ -1661,7 +1682,7 @@
         <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*",B:B, "&lt;&gt;*"&amp;J5&amp;"*")</f>
         <v>100</v>
       </c>
-      <c r="L6" s="69" t="str">
+      <c r="L6" s="72" t="str">
         <f>ROUNDDOWN((K6)/60,0) &amp;":"&amp;(IF(MOD(K6, 60) &lt; 10, "0","")) &amp; MOD(K6,60)</f>
         <v>1:40</v>
       </c>
@@ -1672,25 +1693,25 @@
       <c r="O6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="75"/>
-      <c r="S6" s="38">
+      <c r="P6" s="31"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="41">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O6&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
         <v>990</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="50">
         <v>65</v>
       </c>
       <c r="J7" s="18" t="s">
@@ -1698,40 +1719,21 @@
       </c>
       <c r="K7" s="16">
         <f>SUM(K2:K5)</f>
-        <v>5067</v>
-      </c>
-      <c r="L7" s="69" t="str">
+        <v>6087</v>
+      </c>
+      <c r="L7" s="72" t="str">
         <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
-        <v>84:27</v>
-      </c>
-      <c r="O7" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" s="76">
-        <f>Q3+R3+S3</f>
-        <v>40</v>
-      </c>
-      <c r="Q7" s="76">
-        <f>Q3+R4+S4</f>
-        <v>841</v>
-      </c>
-      <c r="R7" s="72">
-        <f>R3+R4+S5</f>
-        <v>981</v>
-      </c>
-      <c r="S7" s="72">
-        <f>S3+S4+S5</f>
-        <v>580</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+        <v>101:27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="36" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="8">
@@ -1740,34 +1742,15 @@
       <c r="E8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O8" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="76" t="str">
-        <f>ROUNDDOWN((P7)/60,0) &amp;":"&amp;(IF(MOD(P7, 60) &lt; 10, "0","")) &amp; MOD(P7,60)</f>
-        <v>0:40</v>
-      </c>
-      <c r="Q8" s="76" t="str">
-        <f t="shared" ref="Q8:S8" si="1">ROUNDDOWN((Q7)/60,0) &amp;":"&amp;(IF(MOD(Q7, 60) &lt; 10, "0","")) &amp; MOD(Q7,60)</f>
-        <v>14:01</v>
-      </c>
-      <c r="R8" s="76" t="str">
-        <f t="shared" si="1"/>
-        <v>16:21</v>
-      </c>
-      <c r="S8" s="72" t="str">
-        <f t="shared" si="1"/>
-        <v>9:40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="37" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="5">
@@ -1781,7 +1764,7 @@
       <c r="B10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="36" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="8">
@@ -1789,16 +1772,16 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="50">
         <v>60</v>
       </c>
     </row>
@@ -1809,7 +1792,7 @@
       <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="36" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="8">
@@ -1826,164 +1809,164 @@
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="37" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="5">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="37" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="37" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="37" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="5">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="37" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="37" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="37" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="37" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="37" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="50" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="53" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="52" t="s">
         <v>64</v>
       </c>
       <c r="D22" s="7">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="37" t="s">
         <v>51</v>
       </c>
       <c r="D23" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="71" t="s">
+    <row r="24" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="70" t="s">
+      <c r="C24" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="71">
+      <c r="D24" s="74">
         <v>60</v>
       </c>
     </row>
@@ -1994,7 +1977,7 @@
       <c r="B25" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="36" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="8">
@@ -2005,16 +1988,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="51">
+      <c r="D26" s="54">
         <v>40</v>
       </c>
     </row>
@@ -2025,7 +2008,7 @@
       <c r="B27" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="36" t="s">
         <v>72</v>
       </c>
       <c r="D27" s="8">
@@ -2033,287 +2016,287 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="55" t="s">
+      <c r="A28" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="C28" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="58">
+      <c r="D28" s="61">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="55" t="s">
+    <row r="29" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="58">
+      <c r="D29" s="61">
         <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="58">
+      <c r="D30" s="61">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="71" t="s">
+      <c r="B31" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="70" t="s">
+      <c r="C31" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="71">
+      <c r="D31" s="74">
         <v>120</v>
       </c>
-      <c r="E31" s="68"/>
+      <c r="E31" s="71"/>
     </row>
     <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="63" t="s">
+      <c r="A32" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="65" t="s">
+      <c r="B32" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="63">
+      <c r="D32" s="66">
         <v>40</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="63" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
+    <row r="33" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="63">
+      <c r="D33" s="66">
         <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="62" t="s">
+      <c r="A34" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="67" t="s">
+      <c r="C34" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="61">
+      <c r="D34" s="64">
         <v>120</v>
       </c>
-      <c r="E34" s="59"/>
+      <c r="E34" s="62"/>
     </row>
     <row r="35" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="61" t="s">
+      <c r="A35" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="67" t="s">
+      <c r="C35" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="61">
+      <c r="D35" s="64">
         <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="61" t="s">
+      <c r="A36" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="64" t="s">
+      <c r="B36" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="67" t="s">
+      <c r="C36" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="61">
+      <c r="D36" s="64">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="61" t="s">
+    <row r="37" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="64" t="s">
+      <c r="B37" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="61">
+      <c r="D37" s="64">
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="61" t="s">
+    <row r="38" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="64" t="s">
+      <c r="B38" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="67" t="s">
+      <c r="C38" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="61">
+      <c r="D38" s="64">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="62" t="s">
+    <row r="39" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="64" t="s">
+      <c r="B39" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="67" t="s">
+      <c r="C39" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="61">
+      <c r="D39" s="64">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="61" t="s">
+    <row r="40" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="64" t="s">
+      <c r="B40" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="67" t="s">
+      <c r="C40" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="61">
+      <c r="D40" s="64">
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="61" t="s">
+    <row r="41" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="64" t="s">
+      <c r="B41" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="67" t="s">
+      <c r="C41" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="61">
+      <c r="D41" s="64">
         <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="61" t="s">
+      <c r="A42" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="64" t="s">
+      <c r="B42" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="67" t="s">
+      <c r="C42" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="61">
+      <c r="D42" s="64">
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="60" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="61" t="s">
+    <row r="43" spans="1:5" s="63" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="64" t="s">
+      <c r="B43" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="67" t="s">
+      <c r="C43" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="61">
+      <c r="D43" s="64">
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="61" t="s">
+      <c r="A44" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="61" t="s">
+      <c r="B44" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="67" t="s">
+      <c r="C44" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="61">
+      <c r="D44" s="64">
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="60" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="61" t="s">
+    <row r="45" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="67" t="s">
+      <c r="C45" s="70" t="s">
         <v>105</v>
       </c>
-      <c r="D45" s="61">
+      <c r="D45" s="64">
         <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="71" t="s">
+      <c r="A46" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="71" t="s">
+      <c r="B46" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="70" t="s">
+      <c r="C46" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="71">
+      <c r="D46" s="74">
         <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="63" t="s">
+      <c r="A47" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="63" t="s">
+      <c r="B47" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="66" t="s">
+      <c r="C47" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="D47" s="63">
+      <c r="D47" s="66">
         <v>60</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -2321,72 +2304,72 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="61" t="s">
+      <c r="A48" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="61" t="s">
+      <c r="B48" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="67" t="s">
+      <c r="C48" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="61">
+      <c r="D48" s="64">
         <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="61" t="s">
+      <c r="A49" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="67" t="s">
+      <c r="C49" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="61">
+      <c r="D49" s="64">
         <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="43" t="s">
+      <c r="A50" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="65" t="s">
+      <c r="B50" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="66" t="s">
+      <c r="C50" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="D50" s="63">
+      <c r="D50" s="66">
         <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="71" t="s">
+      <c r="A51" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="71" t="s">
+      <c r="B51" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="70" t="s">
+      <c r="C51" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="71">
+      <c r="D51" s="74">
         <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="63" t="s">
+      <c r="A52" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="63" t="s">
+      <c r="B52" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="66" t="s">
+      <c r="C52" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="D52" s="63">
+      <c r="D52" s="66">
         <v>60</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -2394,264 +2377,362 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="43" t="s">
+      <c r="A53" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="65" t="s">
+      <c r="B53" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="66" t="s">
+      <c r="C53" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="63">
+      <c r="D53" s="66">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="6"/>
+    <row r="54" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="66">
+        <v>120</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="6"/>
+      <c r="A55" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="6"/>
+      <c r="A56" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B56" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="70" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="64">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" s="64">
+        <v>120</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="6"/>
+      <c r="A58" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="70" t="s">
+        <v>118</v>
+      </c>
+      <c r="D58" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="35"/>
-      <c r="D60" s="6"/>
+      <c r="A59" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" s="64">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="70" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="6"/>
+      <c r="A61" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="70" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="64">
+        <v>120</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="6"/>
+      <c r="A62" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" s="64">
+        <v>150</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="6"/>
+      <c r="A63" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="70" t="s">
+        <v>126</v>
+      </c>
+      <c r="D63" s="64">
+        <v>120</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="35"/>
+      <c r="C64" s="38"/>
       <c r="D64" s="6"/>
     </row>
     <row r="65" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="35"/>
+      <c r="C65" s="38"/>
       <c r="D65" s="6"/>
     </row>
     <row r="66" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="35"/>
+      <c r="C66" s="38"/>
       <c r="D66" s="6"/>
     </row>
     <row r="67" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="35"/>
+      <c r="C67" s="38"/>
       <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="35"/>
+      <c r="C68" s="38"/>
       <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="35"/>
+      <c r="C69" s="38"/>
       <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="35"/>
+      <c r="C70" s="38"/>
       <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="35"/>
+      <c r="C71" s="38"/>
       <c r="D71" s="6"/>
     </row>
     <row r="72" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="35"/>
+      <c r="C72" s="38"/>
       <c r="D72" s="6"/>
     </row>
     <row r="73" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="35"/>
+      <c r="C73" s="38"/>
       <c r="D73" s="6"/>
     </row>
     <row r="74" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="35"/>
+      <c r="C74" s="38"/>
       <c r="D74" s="6"/>
     </row>
     <row r="75" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="35"/>
+      <c r="C75" s="38"/>
       <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
-      <c r="C76" s="35"/>
+      <c r="C76" s="38"/>
       <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="35"/>
+      <c r="C77" s="38"/>
       <c r="D77" s="6"/>
     </row>
     <row r="78" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="35"/>
+      <c r="C78" s="38"/>
       <c r="D78" s="6"/>
     </row>
     <row r="79" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="35"/>
+      <c r="C79" s="38"/>
       <c r="D79" s="6"/>
     </row>
     <row r="80" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="35"/>
+      <c r="C80" s="38"/>
       <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
-      <c r="C81" s="35"/>
+      <c r="C81" s="38"/>
       <c r="D81" s="6"/>
     </row>
     <row r="82" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
-      <c r="C82" s="35"/>
+      <c r="C82" s="38"/>
       <c r="D82" s="6"/>
     </row>
     <row r="83" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
-      <c r="C83" s="35"/>
+      <c r="C83" s="38"/>
       <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
-      <c r="C84" s="35"/>
+      <c r="C84" s="38"/>
       <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
-      <c r="C85" s="35"/>
+      <c r="C85" s="38"/>
       <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
-      <c r="C86" s="35"/>
+      <c r="C86" s="38"/>
       <c r="D86" s="6"/>
     </row>
     <row r="87" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
-      <c r="C87" s="35"/>
+      <c r="C87" s="38"/>
       <c r="D87" s="6"/>
     </row>
     <row r="88" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
-      <c r="C88" s="35"/>
+      <c r="C88" s="38"/>
       <c r="D88" s="6"/>
     </row>
     <row r="89" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
-      <c r="C89" s="35"/>
+      <c r="C89" s="38"/>
       <c r="D89" s="6"/>
     </row>
     <row r="90" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
-      <c r="C90" s="35"/>
+      <c r="C90" s="38"/>
       <c r="D90" s="6"/>
     </row>
     <row r="91" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
-      <c r="C91" s="35"/>
+      <c r="C91" s="38"/>
       <c r="D91" s="6"/>
     </row>
     <row r="92" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
-      <c r="C92" s="35"/>
+      <c r="C92" s="38"/>
       <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
-      <c r="C93" s="35"/>
+      <c r="C93" s="38"/>
       <c r="D93" s="6"/>
     </row>
     <row r="94" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
-      <c r="C94" s="35"/>
+      <c r="C94" s="38"/>
       <c r="D94" s="6"/>
+    </row>
+    <row r="95" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="6"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="6"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="38"/>
+      <c r="D96" s="6"/>
+    </row>
+    <row r="97" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="6"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="38"/>
+      <c r="D97" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated tasks and schedule
Added extra info for final weeks and some other for previous
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="143">
   <si>
     <t>Worked by:</t>
   </si>
@@ -398,6 +398,54 @@
   </si>
   <si>
     <t>19.04. || 12:00</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>20.04. || 10:30</t>
+  </si>
+  <si>
+    <t>21.04. || 12:00</t>
+  </si>
+  <si>
+    <t>22.04. || 13:30</t>
+  </si>
+  <si>
+    <t>Database SQL</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>23.04. || 20:00</t>
+  </si>
+  <si>
+    <t>23.04. || 22:00</t>
+  </si>
+  <si>
+    <t>Setup document review</t>
+  </si>
+  <si>
+    <t>23.04. || 21:00</t>
+  </si>
+  <si>
+    <t>23.04. || 19:00</t>
+  </si>
+  <si>
+    <t>23.04. || 19:30</t>
+  </si>
+  <si>
+    <t>Schedule and website review</t>
+  </si>
+  <si>
+    <t>Georgi and Angel</t>
+  </si>
+  <si>
+    <t>24.04. || 11:30</t>
+  </si>
+  <si>
+    <t>24.04. || 12:40</t>
   </si>
 </sst>
 </file>
@@ -1429,10 +1477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S97"/>
+  <dimension ref="A1:S100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,15 +1547,15 @@
       </c>
       <c r="K2" s="23">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
-        <v>1090</v>
+        <v>1420</v>
       </c>
       <c r="L2" s="72" t="str">
         <f t="shared" ref="L2:L5" si="0">ROUNDDOWN((K2)/60,0) &amp;":"&amp;(IF(MOD(K2, 60) &lt; 10, "0","")) &amp; MOD(K2,60)</f>
-        <v>18:10</v>
+        <v>23:40</v>
       </c>
       <c r="M2" s="17" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>18%</v>
+        <v>21%</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>15</v>
@@ -1543,11 +1591,11 @@
       </c>
       <c r="K3" s="16">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>1591</v>
+        <v>1761</v>
       </c>
       <c r="L3" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>26:31</v>
+        <v>29:21</v>
       </c>
       <c r="M3" s="17" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
@@ -1558,11 +1606,11 @@
       </c>
       <c r="P3" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
-        <v>1090</v>
+        <v>1420</v>
       </c>
       <c r="Q3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="R3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
@@ -1592,15 +1640,15 @@
       </c>
       <c r="K4" s="16">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>2416</v>
+        <v>2656</v>
       </c>
       <c r="L4" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>40:16</v>
+        <v>44:16</v>
       </c>
       <c r="M4" s="17" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>40%</v>
+        <v>39%</v>
       </c>
       <c r="O4" s="28" t="s">
         <v>9</v>
@@ -1608,7 +1656,7 @@
       <c r="P4" s="27"/>
       <c r="Q4" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>1591</v>
+        <v>1761</v>
       </c>
       <c r="R4" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
@@ -1645,7 +1693,7 @@
       </c>
       <c r="M5" s="17" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>16%</v>
+        <v>15%</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>7</v>
@@ -1654,7 +1702,7 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>2416</v>
+        <v>2656</v>
       </c>
       <c r="S5" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1680,15 +1728,15 @@
       </c>
       <c r="K6" s="20">
         <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*",B:B, "&lt;&gt;*"&amp;J5&amp;"*")</f>
-        <v>100</v>
+        <v>385</v>
       </c>
       <c r="L6" s="72" t="str">
         <f>ROUNDDOWN((K6)/60,0) &amp;":"&amp;(IF(MOD(K6, 60) &lt; 10, "0","")) &amp; MOD(K6,60)</f>
-        <v>1:40</v>
+        <v>6:25</v>
       </c>
       <c r="M6" s="21" t="str">
         <f>ROUND(($K$6) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>2%</v>
+        <v>6%</v>
       </c>
       <c r="O6" s="29" t="s">
         <v>13</v>
@@ -1719,11 +1767,11 @@
       </c>
       <c r="K7" s="16">
         <f>SUM(K2:K5)</f>
-        <v>6087</v>
+        <v>6827</v>
       </c>
       <c r="L7" s="72" t="str">
         <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
-        <v>101:27</v>
+        <v>113:47</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2516,79 +2564,162 @@
         <v>150</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="65" t="s">
+    <row r="63" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="B63" s="64" t="s">
+      <c r="B63" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="70" t="s">
+      <c r="C63" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="D63" s="64">
+      <c r="D63" s="74">
         <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="6"/>
+      <c r="A64" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="D64" s="66">
+        <v>165</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="65" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="6"/>
+      <c r="A65" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="64">
+        <v>120</v>
+      </c>
     </row>
     <row r="66" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="6"/>
-    </row>
-    <row r="67" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="6"/>
-    </row>
-    <row r="68" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="6"/>
-    </row>
-    <row r="69" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="6"/>
+      <c r="A66" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="D66" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" s="64">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="B68" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" s="64">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="64" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D69" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="70" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="38"/>
-      <c r="D70" s="6"/>
+      <c r="A70" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B70" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="D70" s="64">
+        <v>120</v>
+      </c>
     </row>
     <row r="71" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="6"/>
+      <c r="A71" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D71" s="64">
+        <v>120</v>
+      </c>
     </row>
     <row r="72" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="6"/>
+      <c r="A72" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="64" t="s">
+        <v>140</v>
+      </c>
+      <c r="C72" s="70" t="s">
+        <v>141</v>
+      </c>
+      <c r="D72" s="64">
+        <v>80</v>
+      </c>
     </row>
     <row r="73" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="6"/>
+      <c r="A73" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B73" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="D73" s="64">
+        <v>30</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
@@ -2734,6 +2865,24 @@
       <c r="C97" s="38"/>
       <c r="D97" s="6"/>
     </row>
+    <row r="98" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="6"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="38"/>
+      <c r="D98" s="6"/>
+    </row>
+    <row r="99" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="6"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="38"/>
+      <c r="D99" s="6"/>
+    </row>
+    <row r="100" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="38"/>
+      <c r="D100" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated tasks for week 11
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="186">
   <si>
     <t>Worked by:</t>
   </si>
@@ -481,9 +481,6 @@
     <t>23.04. || 13:00</t>
   </si>
   <si>
-    <t>16.04. || 11:00</t>
-  </si>
-  <si>
     <t>13.04. || 16:30</t>
   </si>
   <si>
@@ -542,6 +539,42 @@
   </si>
   <si>
     <t>08.05. || 12:00</t>
+  </si>
+  <si>
+    <t>06.05. || 14:00</t>
+  </si>
+  <si>
+    <t>08.05. || 13:00</t>
+  </si>
+  <si>
+    <t>09.05. || 13:00</t>
+  </si>
+  <si>
+    <t>10.05. || 13:00</t>
+  </si>
+  <si>
+    <t>PHP ticket func</t>
+  </si>
+  <si>
+    <t>Angel and Ilia</t>
+  </si>
+  <si>
+    <t>11.05. || 11:00</t>
+  </si>
+  <si>
+    <t>11.05. || 12:00</t>
+  </si>
+  <si>
+    <t>Database review and foreign key structure</t>
+  </si>
+  <si>
+    <t>07.05. || 12:00</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t>09.05. || 18:00</t>
   </si>
 </sst>
 </file>
@@ -1573,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S109"/>
+  <dimension ref="A1:S111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,15 +1676,15 @@
       </c>
       <c r="K2" s="23">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
-        <v>2260</v>
+        <v>2920</v>
       </c>
       <c r="L2" s="72" t="str">
         <f t="shared" ref="L2:L5" si="0">ROUNDDOWN((K2)/60,0) &amp;":"&amp;(IF(MOD(K2, 60) &lt; 10, "0","")) &amp; MOD(K2,60)</f>
-        <v>37:40</v>
+        <v>48:40</v>
       </c>
       <c r="M2" s="17" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>23%</v>
+        <v>27%</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>15</v>
@@ -1687,22 +1720,22 @@
       </c>
       <c r="K3" s="16">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>2221</v>
+        <v>2541</v>
       </c>
       <c r="L3" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>37:01</v>
+        <v>42:21</v>
       </c>
       <c r="M3" s="17" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>23%</v>
+        <v>24%</v>
       </c>
       <c r="O3" s="30" t="s">
         <v>15</v>
       </c>
       <c r="P3" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
-        <v>2260</v>
+        <v>2920</v>
       </c>
       <c r="Q3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
@@ -1710,7 +1743,7 @@
       </c>
       <c r="R3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="S3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1736,15 +1769,15 @@
       </c>
       <c r="K4" s="16">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>2991</v>
+        <v>3111</v>
       </c>
       <c r="L4" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>49:51</v>
+        <v>51:51</v>
       </c>
       <c r="M4" s="17" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>31%</v>
+        <v>29%</v>
       </c>
       <c r="O4" s="28" t="s">
         <v>9</v>
@@ -1752,7 +1785,7 @@
       <c r="P4" s="27"/>
       <c r="Q4" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>2221</v>
+        <v>2541</v>
       </c>
       <c r="R4" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
@@ -1781,15 +1814,15 @@
       </c>
       <c r="K5" s="16">
         <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
-        <v>2310</v>
+        <v>2070</v>
       </c>
       <c r="L5" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>38:30</v>
+        <v>34:30</v>
       </c>
       <c r="M5" s="17" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>24%</v>
+        <v>19%</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>7</v>
@@ -1798,7 +1831,7 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>2991</v>
+        <v>3111</v>
       </c>
       <c r="S5" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1832,7 +1865,7 @@
       </c>
       <c r="M6" s="21" t="str">
         <f>ROUND(($K$6) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>5%</v>
+        <v>4%</v>
       </c>
       <c r="O6" s="29" t="s">
         <v>13</v>
@@ -1842,7 +1875,7 @@
       <c r="R6" s="33"/>
       <c r="S6" s="41">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O6&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
-        <v>2310</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1863,11 +1896,11 @@
       </c>
       <c r="K7" s="16">
         <f>SUM(K2:K5)</f>
-        <v>9782</v>
+        <v>10642</v>
       </c>
       <c r="L7" s="72" t="str">
         <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
-        <v>163:02</v>
+        <v>177:22</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2542,7 +2575,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="69" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D54" s="66">
         <v>180</v>
@@ -2592,391 +2625,391 @@
     </row>
     <row r="58" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="64" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="B58" s="64" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C58" s="70" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="D58" s="64">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="64" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B59" s="64" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C59" s="70" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D59" s="64">
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="64" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="B60" s="64" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C60" s="70" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D60" s="64">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="64" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="B61" s="64" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="70" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D61" s="64">
-        <v>180</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="64" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B62" s="64" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C62" s="70" t="s">
         <v>122</v>
       </c>
       <c r="D62" s="64">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="64" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="B63" s="64" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C63" s="70" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D63" s="64">
-        <v>180</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="64" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B64" s="64" t="s">
         <v>7</v>
       </c>
       <c r="C64" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" s="64">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="60" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65" s="61">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" s="74">
         <v>120</v>
       </c>
-      <c r="D64" s="64">
+    </row>
+    <row r="67" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" s="66">
+        <v>165</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="69" t="s">
+        <v>151</v>
+      </c>
+      <c r="D68" s="66">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="64">
         <v>120</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="B65" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" s="70" t="s">
-        <v>124</v>
-      </c>
-      <c r="D65" s="64">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="B66" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66" s="60" t="s">
-        <v>156</v>
-      </c>
-      <c r="D66" s="61">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="B67" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="C67" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="D67" s="74">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68" s="66" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="69" t="s">
-        <v>128</v>
-      </c>
-      <c r="D68" s="66">
-        <v>165</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="66" t="s">
-        <v>87</v>
-      </c>
-      <c r="B69" s="66" t="s">
-        <v>13</v>
-      </c>
-      <c r="C69" s="69" t="s">
-        <v>151</v>
-      </c>
-      <c r="D69" s="66">
-        <v>180</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="64" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B70" s="64" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C70" s="70" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D70" s="64">
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="64" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="B71" s="64" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C71" s="70" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D71" s="64">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="64" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B72" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C72" s="70" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D72" s="64">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="64" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="B73" s="64" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C73" s="70" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D73" s="64">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="64" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B74" s="64" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C74" s="70" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D74" s="64">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="64" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="B75" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="70" t="s">
+        <v>153</v>
+      </c>
+      <c r="D75" s="64">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="70" t="s">
-        <v>133</v>
-      </c>
-      <c r="D75" s="64">
+      <c r="C76" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D76" s="64">
         <v>120</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="B76" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="C76" s="70" t="s">
-        <v>153</v>
-      </c>
-      <c r="D76" s="64">
-        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="64" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B77" s="64" t="s">
-        <v>7</v>
+        <v>140</v>
       </c>
       <c r="C77" s="70" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="D77" s="64">
-        <v>120</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="64" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="B78" s="64" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C78" s="70" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D78" s="64">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="64" t="s">
-        <v>101</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="65" t="s">
+        <v>143</v>
       </c>
       <c r="B79" s="64" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C79" s="70" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D79" s="64">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="65" t="s">
-        <v>143</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="64" t="s">
+        <v>144</v>
       </c>
       <c r="B80" s="64" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C80" s="70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D80" s="64">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="64" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B81" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="D81" s="64">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="B82" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C81" s="70" t="s">
-        <v>145</v>
-      </c>
-      <c r="D81" s="64">
+      <c r="C82" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="D82" s="74">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="69" t="s">
+        <v>156</v>
+      </c>
+      <c r="D83" s="66">
         <v>60</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="B82" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C82" s="70" t="s">
-        <v>148</v>
-      </c>
-      <c r="D82" s="64">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="74" t="s">
-        <v>149</v>
-      </c>
-      <c r="B83" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="C83" s="73" t="s">
-        <v>150</v>
-      </c>
-      <c r="D83" s="74">
-        <v>180</v>
+      <c r="E83" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="B84" s="68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C84" s="69" t="s">
-        <v>157</v>
-      </c>
-      <c r="D84" s="66">
-        <v>60</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>152</v>
+      <c r="A84" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="B84" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="D84" s="64">
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B85" s="64" t="s">
         <v>15</v>
@@ -2988,37 +3021,37 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="64" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B86" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="D86" s="64">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="B87" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C86" s="70" t="s">
+      <c r="C87" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="D86" s="64">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="64" t="s">
-        <v>166</v>
-      </c>
-      <c r="B87" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C87" s="70" t="s">
-        <v>167</v>
-      </c>
       <c r="D87" s="64">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B88" s="64" t="s">
         <v>15</v>
@@ -3027,198 +3060,269 @@
         <v>163</v>
       </c>
       <c r="D88" s="64">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="64" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B89" s="64" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C89" s="70" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D89" s="64">
-        <v>240</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="64" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B90" s="64" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C90" s="70" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D90" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="64" t="s">
+        <v>169</v>
+      </c>
+      <c r="B91" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="D91" s="64">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="64" t="s">
+        <v>157</v>
+      </c>
+      <c r="B92" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="C92" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="D92" s="64">
         <v>60</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="64" t="s">
-        <v>160</v>
-      </c>
-      <c r="B91" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="C91" s="70" t="s">
-        <v>165</v>
-      </c>
-      <c r="D91" s="64">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="64" t="s">
-        <v>170</v>
-      </c>
-      <c r="B92" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" s="70" t="s">
-        <v>171</v>
-      </c>
-      <c r="D92" s="64">
-        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="64" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B93" s="64" t="s">
-        <v>168</v>
+        <v>7</v>
       </c>
       <c r="C93" s="70" t="s">
+        <v>171</v>
+      </c>
+      <c r="D93" s="64">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="B94" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="D94" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="64" t="s">
         <v>169</v>
-      </c>
-      <c r="D93" s="64">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="64" t="s">
-        <v>144</v>
-      </c>
-      <c r="B94" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" s="70" t="s">
-        <v>172</v>
-      </c>
-      <c r="D94" s="64">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="64" t="s">
-        <v>170</v>
       </c>
       <c r="B95" s="64" t="s">
         <v>7</v>
       </c>
       <c r="C95" s="70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D95" s="64">
         <v>50</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="46" t="s">
+      <c r="A96" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="B96" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="70" t="s">
+        <v>183</v>
+      </c>
+      <c r="D96" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B96" s="68" t="s">
+      <c r="B97" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C96" s="69" t="s">
-        <v>174</v>
-      </c>
-      <c r="D96" s="66">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="6"/>
-      <c r="B97" s="6"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="6"/>
-    </row>
-    <row r="98" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="6"/>
-      <c r="B98" s="6"/>
-      <c r="C98" s="38"/>
-      <c r="D98" s="6"/>
-    </row>
-    <row r="99" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6"/>
-      <c r="C99" s="38"/>
-      <c r="D99" s="6"/>
-    </row>
-    <row r="100" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6"/>
-      <c r="C100" s="38"/>
-      <c r="D100" s="6"/>
-    </row>
-    <row r="101" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="6"/>
-      <c r="B101" s="6"/>
-      <c r="C101" s="38"/>
-      <c r="D101" s="6"/>
-    </row>
-    <row r="102" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="6"/>
-      <c r="B102" s="6"/>
-      <c r="C102" s="38"/>
-      <c r="D102" s="6"/>
-    </row>
-    <row r="103" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="6"/>
-      <c r="B103" s="6"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="6"/>
-    </row>
-    <row r="104" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="D97" s="66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="B98" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="D98" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="D99" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="D100" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="73" t="s">
+        <v>177</v>
+      </c>
+      <c r="D101" s="74">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="66" t="s">
+        <v>178</v>
+      </c>
+      <c r="B102" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" s="69" t="s">
+        <v>180</v>
+      </c>
+      <c r="D102" s="66">
+        <v>120</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" s="69" t="s">
+        <v>181</v>
+      </c>
+      <c r="D103" s="66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="38"/>
       <c r="D104" s="6"/>
     </row>
-    <row r="105" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="38"/>
       <c r="D105" s="6"/>
     </row>
-    <row r="106" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="38"/>
       <c r="D106" s="6"/>
     </row>
-    <row r="107" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="38"/>
       <c r="D107" s="6"/>
     </row>
-    <row r="108" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="38"/>
       <c r="D108" s="6"/>
     </row>
-    <row r="109" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="38"/>
       <c r="D109" s="6"/>
+    </row>
+    <row r="110" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="6"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="38"/>
+      <c r="D110" s="6"/>
+    </row>
+    <row r="111" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="6"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="38"/>
+      <c r="D111" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Documentation updates and GUI for renting and appointments
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="193">
   <si>
     <t>Worked by:</t>
   </si>
@@ -575,6 +575,27 @@
   </si>
   <si>
     <t>09.05. || 18:00</t>
+  </si>
+  <si>
+    <t>12.05. || 19:00</t>
+  </si>
+  <si>
+    <t>12.05. || 20:00</t>
+  </si>
+  <si>
+    <t>Database to class conversion</t>
+  </si>
+  <si>
+    <t>14.05. || 21:00</t>
+  </si>
+  <si>
+    <t>RFID</t>
+  </si>
+  <si>
+    <t>12.05. || 16:00</t>
+  </si>
+  <si>
+    <t>14.05. || 16:00</t>
   </si>
 </sst>
 </file>
@@ -1606,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S111"/>
+  <dimension ref="A1:S112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,11 +1697,11 @@
       </c>
       <c r="K2" s="23">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
-        <v>2920</v>
+        <v>3100</v>
       </c>
       <c r="L2" s="72" t="str">
         <f t="shared" ref="L2:L5" si="0">ROUNDDOWN((K2)/60,0) &amp;":"&amp;(IF(MOD(K2, 60) &lt; 10, "0","")) &amp; MOD(K2,60)</f>
-        <v>48:40</v>
+        <v>51:40</v>
       </c>
       <c r="M2" s="17" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
@@ -1720,11 +1741,11 @@
       </c>
       <c r="K3" s="16">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>2541</v>
+        <v>2721</v>
       </c>
       <c r="L3" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>42:21</v>
+        <v>45:21</v>
       </c>
       <c r="M3" s="17" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
@@ -1735,15 +1756,15 @@
       </c>
       <c r="P3" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
-        <v>2920</v>
+        <v>3100</v>
       </c>
       <c r="Q3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="R3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="S3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1769,15 +1790,15 @@
       </c>
       <c r="K4" s="16">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>3111</v>
+        <v>3591</v>
       </c>
       <c r="L4" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>51:51</v>
+        <v>59:51</v>
       </c>
       <c r="M4" s="17" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>29%</v>
+        <v>31%</v>
       </c>
       <c r="O4" s="28" t="s">
         <v>9</v>
@@ -1785,11 +1806,11 @@
       <c r="P4" s="27"/>
       <c r="Q4" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>2541</v>
+        <v>2721</v>
       </c>
       <c r="R4" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>721</v>
+        <v>841</v>
       </c>
       <c r="S4" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1822,7 +1843,7 @@
       </c>
       <c r="M5" s="17" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>19%</v>
+        <v>18%</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>7</v>
@@ -1831,7 +1852,7 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>3111</v>
+        <v>3591</v>
       </c>
       <c r="S5" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1896,11 +1917,11 @@
       </c>
       <c r="K7" s="16">
         <f>SUM(K2:K5)</f>
-        <v>10642</v>
+        <v>11482</v>
       </c>
       <c r="L7" s="72" t="str">
         <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
-        <v>177:22</v>
+        <v>191:22</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3276,35 +3297,75 @@
         <v>60</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="6"/>
-      <c r="B104" s="6"/>
-      <c r="C104" s="38"/>
-      <c r="D104" s="6"/>
+    <row r="104" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="B104" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="D104" s="66">
+        <v>180</v>
+      </c>
     </row>
     <row r="105" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="6"/>
-      <c r="B105" s="6"/>
-      <c r="C105" s="38"/>
-      <c r="D105" s="6"/>
+      <c r="A105" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="B105" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="D105" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="106" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="6"/>
-      <c r="B106" s="6"/>
-      <c r="C106" s="38"/>
-      <c r="D106" s="6"/>
+      <c r="A106" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="B106" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="C106" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="D106" s="64">
+        <v>120</v>
+      </c>
     </row>
     <row r="107" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="6"/>
-      <c r="B107" s="6"/>
-      <c r="C107" s="38"/>
-      <c r="D107" s="6"/>
+      <c r="A107" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" s="70" t="s">
+        <v>192</v>
+      </c>
+      <c r="D107" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="108" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="6"/>
-      <c r="B108" s="6"/>
-      <c r="C108" s="38"/>
-      <c r="D108" s="6"/>
+      <c r="A108" s="64" t="s">
+        <v>188</v>
+      </c>
+      <c r="B108" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="D108" s="64">
+        <v>180</v>
+      </c>
     </row>
     <row r="109" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
@@ -3324,6 +3385,12 @@
       <c r="C111" s="38"/>
       <c r="D111" s="6"/>
     </row>
+    <row r="112" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="6"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="38"/>
+      <c r="D112" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Documentation and Rent GUI
Ignore Program.cs
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="246">
   <si>
     <t>Worked by:</t>
   </si>
@@ -662,6 +662,99 @@
   </si>
   <si>
     <t>19.05. || 21:00</t>
+  </si>
+  <si>
+    <t>Ticket functionality</t>
+  </si>
+  <si>
+    <t>20.05. || 21:00</t>
+  </si>
+  <si>
+    <t>22.05. || 12:00</t>
+  </si>
+  <si>
+    <t>Ticket and twitter func</t>
+  </si>
+  <si>
+    <t>29.05. || 00:00</t>
+  </si>
+  <si>
+    <t>GUI issues</t>
+  </si>
+  <si>
+    <t>Booking application</t>
+  </si>
+  <si>
+    <t>28.05. || 20:00</t>
+  </si>
+  <si>
+    <t>Booking overview</t>
+  </si>
+  <si>
+    <t>28.05. || 13:30</t>
+  </si>
+  <si>
+    <t>Database logging</t>
+  </si>
+  <si>
+    <t>27.05. || 13:00</t>
+  </si>
+  <si>
+    <t>Renting logic</t>
+  </si>
+  <si>
+    <t>31.05. || 16:00</t>
+  </si>
+  <si>
+    <t>28.05. || 12:00</t>
+  </si>
+  <si>
+    <t>20.05. || 00:00</t>
+  </si>
+  <si>
+    <t>26.05. || 12:00</t>
+  </si>
+  <si>
+    <t>24.05. || 16:00</t>
+  </si>
+  <si>
+    <t>Application division</t>
+  </si>
+  <si>
+    <t>Search at shops</t>
+  </si>
+  <si>
+    <t>Website paypal doc</t>
+  </si>
+  <si>
+    <t>25.05. || 12:00</t>
+  </si>
+  <si>
+    <t>20.05. || 20:00</t>
+  </si>
+  <si>
+    <t>C# Admin GUI</t>
+  </si>
+  <si>
+    <t>18.05. || 15:00</t>
+  </si>
+  <si>
+    <t>24.05. || 20:00</t>
+  </si>
+  <si>
+    <t>Week 14</t>
+  </si>
+  <si>
+    <t>Classes Integrity</t>
+  </si>
+  <si>
+    <t>Database Integrity</t>
+  </si>
+  <si>
+    <t>26.05. || 13:00</t>
+  </si>
+  <si>
+    <t>26.05. || 18:30</t>
   </si>
 </sst>
 </file>
@@ -1693,10 +1786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S188"/>
+  <dimension ref="A1:S202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122:D122"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,15 +1856,15 @@
       </c>
       <c r="K2" s="23">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
-        <v>3280</v>
+        <v>3460</v>
       </c>
       <c r="L2" s="72" t="str">
         <f t="shared" ref="L2:L5" si="0">ROUNDDOWN((K2)/60,0) &amp;":"&amp;(IF(MOD(K2, 60) &lt; 10, "0","")) &amp; MOD(K2,60)</f>
-        <v>54:40</v>
+        <v>57:40</v>
       </c>
       <c r="M2" s="17" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>27%</v>
+        <v>24%</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>15</v>
@@ -1807,22 +1900,22 @@
       </c>
       <c r="K3" s="16">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>3171</v>
+        <v>3591</v>
       </c>
       <c r="L3" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>52:51</v>
+        <v>59:51</v>
       </c>
       <c r="M3" s="17" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>26%</v>
+        <v>25%</v>
       </c>
       <c r="O3" s="30" t="s">
         <v>15</v>
       </c>
       <c r="P3" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;P$2&amp;"*"))</f>
-        <v>3280</v>
+        <v>3460</v>
       </c>
       <c r="Q3" s="35">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O3&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
@@ -1856,11 +1949,11 @@
       </c>
       <c r="K4" s="16">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>3776</v>
+        <v>4496</v>
       </c>
       <c r="L4" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>62:56</v>
+        <v>74:56</v>
       </c>
       <c r="M4" s="17" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
@@ -1872,7 +1965,7 @@
       <c r="P4" s="27"/>
       <c r="Q4" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>3171</v>
+        <v>3591</v>
       </c>
       <c r="R4" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
@@ -1901,15 +1994,15 @@
       </c>
       <c r="K5" s="16">
         <f>(SUMIF(B:B, "*"&amp;J5&amp;"*",D:D ))</f>
-        <v>2130</v>
+        <v>3010</v>
       </c>
       <c r="L5" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>35:30</v>
+        <v>50:10</v>
       </c>
       <c r="M5" s="17" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>17%</v>
+        <v>21%</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>7</v>
@@ -1918,7 +2011,7 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>3776</v>
+        <v>4496</v>
       </c>
       <c r="S5" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -1952,7 +2045,7 @@
       </c>
       <c r="M6" s="21" t="str">
         <f>ROUND(($K$6) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>8%</v>
+        <v>7%</v>
       </c>
       <c r="O6" s="29" t="s">
         <v>13</v>
@@ -1962,7 +2055,7 @@
       <c r="R6" s="33"/>
       <c r="S6" s="41">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O6&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
-        <v>2130</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1983,11 +2076,11 @@
       </c>
       <c r="K7" s="16">
         <f>SUM(K2:K5)</f>
-        <v>12357</v>
+        <v>14557</v>
       </c>
       <c r="L7" s="72" t="str">
         <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
-        <v>205:57</v>
+        <v>242:37</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3562,203 +3655,350 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="64" t="s">
+    <row r="118" spans="1:5" s="63" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="46" t="s">
+        <v>238</v>
+      </c>
+      <c r="B118" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C118" s="69" t="s">
+        <v>239</v>
+      </c>
+      <c r="D118" s="66">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="64" t="s">
         <v>193</v>
-      </c>
-      <c r="B118" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C118" s="70" t="s">
-        <v>194</v>
-      </c>
-      <c r="D118" s="64">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="64" t="s">
-        <v>195</v>
       </c>
       <c r="B119" s="64" t="s">
         <v>7</v>
       </c>
       <c r="C119" s="70" t="s">
+        <v>194</v>
+      </c>
+      <c r="D119" s="64">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="64" t="s">
+        <v>195</v>
+      </c>
+      <c r="B120" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="70" t="s">
         <v>196</v>
       </c>
-      <c r="D119" s="64">
+      <c r="D120" s="64">
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="46" t="s">
+    <row r="121" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="B120" s="68" t="s">
+      <c r="B121" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C120" s="69" t="s">
+      <c r="C121" s="69" t="s">
         <v>211</v>
       </c>
-      <c r="D120" s="66">
+      <c r="D121" s="66">
         <v>60</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="64" t="s">
-        <v>212</v>
-      </c>
-      <c r="B121" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C121" s="70" t="s">
-        <v>213</v>
-      </c>
-      <c r="D121" s="64">
-        <v>120</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="64" t="s">
-        <v>66</v>
+        <v>212</v>
       </c>
       <c r="B122" s="64" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C122" s="70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D122" s="64">
         <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="6"/>
-      <c r="B123" s="6"/>
-      <c r="C123" s="38"/>
-      <c r="D123" s="6"/>
-    </row>
-    <row r="124" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="6"/>
-      <c r="B124" s="6"/>
-      <c r="C124" s="38"/>
-      <c r="D124" s="6"/>
-    </row>
-    <row r="125" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="6"/>
-      <c r="B125" s="6"/>
-      <c r="C125" s="38"/>
-      <c r="D125" s="6"/>
+      <c r="A123" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B123" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="D123" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="B124" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C124" s="70" t="s">
+        <v>237</v>
+      </c>
+      <c r="D124" s="64">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="64" t="s">
+        <v>193</v>
+      </c>
+      <c r="B125" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="D125" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="126" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="6"/>
-      <c r="B126" s="6"/>
-      <c r="C126" s="38"/>
-      <c r="D126" s="6"/>
+      <c r="A126" s="64" t="s">
+        <v>215</v>
+      </c>
+      <c r="B126" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" s="70" t="s">
+        <v>216</v>
+      </c>
+      <c r="D126" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="127" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="6"/>
-      <c r="B127" s="6"/>
-      <c r="C127" s="38"/>
-      <c r="D127" s="6"/>
-    </row>
-    <row r="128" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="6"/>
-      <c r="B128" s="6"/>
-      <c r="C128" s="38"/>
-      <c r="D128" s="6"/>
-    </row>
-    <row r="129" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="6"/>
-      <c r="B129" s="6"/>
-      <c r="C129" s="38"/>
-      <c r="D129" s="6"/>
-    </row>
-    <row r="130" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="6"/>
-      <c r="B130" s="6"/>
-      <c r="C130" s="38"/>
-      <c r="D130" s="6"/>
-    </row>
-    <row r="131" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="6"/>
-      <c r="B131" s="6"/>
-      <c r="C131" s="38"/>
-      <c r="D131" s="6"/>
-    </row>
-    <row r="132" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="6"/>
-      <c r="B132" s="6"/>
-      <c r="C132" s="38"/>
-      <c r="D132" s="6"/>
-    </row>
-    <row r="133" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="6"/>
-      <c r="B133" s="6"/>
-      <c r="C133" s="38"/>
-      <c r="D133" s="6"/>
-    </row>
-    <row r="134" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="6"/>
-      <c r="B134" s="6"/>
-      <c r="C134" s="38"/>
-      <c r="D134" s="6"/>
-    </row>
-    <row r="135" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="6"/>
-      <c r="B135" s="6"/>
-      <c r="C135" s="38"/>
-      <c r="D135" s="6"/>
-    </row>
-    <row r="136" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="6"/>
-      <c r="B136" s="6"/>
-      <c r="C136" s="38"/>
-      <c r="D136" s="6"/>
-    </row>
-    <row r="137" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="6"/>
-      <c r="B137" s="6"/>
-      <c r="C137" s="38"/>
-      <c r="D137" s="6"/>
-    </row>
-    <row r="138" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="6"/>
-      <c r="B138" s="6"/>
-      <c r="C138" s="38"/>
-      <c r="D138" s="6"/>
-    </row>
-    <row r="139" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="6"/>
-      <c r="B139" s="6"/>
-      <c r="C139" s="38"/>
-      <c r="D139" s="6"/>
-    </row>
-    <row r="140" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="6"/>
-      <c r="B140" s="6"/>
-      <c r="C140" s="38"/>
-      <c r="D140" s="6"/>
-    </row>
-    <row r="141" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="64" t="s">
+        <v>218</v>
+      </c>
+      <c r="B127" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="D127" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="64" t="s">
+        <v>225</v>
+      </c>
+      <c r="B128" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="D128" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B129" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129" s="73" t="s">
+        <v>205</v>
+      </c>
+      <c r="D129" s="74">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="B130" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130" s="69" t="s">
+        <v>240</v>
+      </c>
+      <c r="D130" s="66">
+        <v>30</v>
+      </c>
+      <c r="E130" s="63" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="B131" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C131" s="69" t="s">
+        <v>232</v>
+      </c>
+      <c r="D131" s="66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="B132" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" s="69" t="s">
+        <v>231</v>
+      </c>
+      <c r="D132" s="66">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="B133" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C133" s="69" t="s">
+        <v>236</v>
+      </c>
+      <c r="D133" s="66">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="B134" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134" s="69" t="s">
+        <v>244</v>
+      </c>
+      <c r="D134" s="66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="B135" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="D135" s="66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="64" t="s">
+        <v>223</v>
+      </c>
+      <c r="B136" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="70" t="s">
+        <v>224</v>
+      </c>
+      <c r="D136" s="64">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="64" t="s">
+        <v>201</v>
+      </c>
+      <c r="B137" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" s="70" t="s">
+        <v>229</v>
+      </c>
+      <c r="D137" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" s="63" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="64" t="s">
+        <v>221</v>
+      </c>
+      <c r="B138" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C138" s="70" t="s">
+        <v>222</v>
+      </c>
+      <c r="D138" s="64">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="B139" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="D139" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="64" t="s">
+        <v>227</v>
+      </c>
+      <c r="B140" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" s="70" t="s">
+        <v>228</v>
+      </c>
+      <c r="D140" s="64">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6"/>
       <c r="B141" s="6"/>
       <c r="C141" s="38"/>
       <c r="D141" s="6"/>
     </row>
-    <row r="142" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="C142" s="38"/>
       <c r="D142" s="6"/>
     </row>
-    <row r="143" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6"/>
       <c r="B143" s="6"/>
       <c r="C143" s="38"/>
       <c r="D143" s="6"/>
     </row>
-    <row r="144" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6"/>
       <c r="B144" s="6"/>
       <c r="C144" s="38"/>
@@ -4028,6 +4268,90 @@
       <c r="C188" s="38"/>
       <c r="D188" s="6"/>
     </row>
+    <row r="189" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="6"/>
+      <c r="B189" s="6"/>
+      <c r="C189" s="38"/>
+      <c r="D189" s="6"/>
+    </row>
+    <row r="190" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="6"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="38"/>
+      <c r="D190" s="6"/>
+    </row>
+    <row r="191" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="6"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="38"/>
+      <c r="D191" s="6"/>
+    </row>
+    <row r="192" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="6"/>
+      <c r="B192" s="6"/>
+      <c r="C192" s="38"/>
+      <c r="D192" s="6"/>
+    </row>
+    <row r="193" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="6"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="38"/>
+      <c r="D193" s="6"/>
+    </row>
+    <row r="194" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="6"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="38"/>
+      <c r="D194" s="6"/>
+    </row>
+    <row r="195" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="6"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="38"/>
+      <c r="D195" s="6"/>
+    </row>
+    <row r="196" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="6"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="38"/>
+      <c r="D196" s="6"/>
+    </row>
+    <row r="197" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="38"/>
+      <c r="D197" s="6"/>
+    </row>
+    <row r="198" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="6"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="38"/>
+      <c r="D198" s="6"/>
+    </row>
+    <row r="199" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="6"/>
+      <c r="B199" s="6"/>
+      <c r="C199" s="38"/>
+      <c r="D199" s="6"/>
+    </row>
+    <row r="200" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="6"/>
+      <c r="B200" s="6"/>
+      <c r="C200" s="38"/>
+      <c r="D200" s="6"/>
+    </row>
+    <row r="201" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="6"/>
+      <c r="B201" s="6"/>
+      <c r="C201" s="38"/>
+      <c r="D201" s="6"/>
+    </row>
+    <row r="202" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="6"/>
+      <c r="B202" s="6"/>
+      <c r="C202" s="38"/>
+      <c r="D202" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
+ Logged IN @ visitors Prorcess report 9,10,11
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$47</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="256">
   <si>
     <t>Worked by:</t>
   </si>
@@ -755,6 +755,36 @@
   </si>
   <si>
     <t>26.05. || 18:30</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>01.06 || 02:00</t>
+  </si>
+  <si>
+    <t>Classes functionality</t>
+  </si>
+  <si>
+    <t>04.06 || 02:00</t>
+  </si>
+  <si>
+    <t>Database Helpers fixes</t>
+  </si>
+  <si>
+    <t>06.06 || 22:00</t>
+  </si>
+  <si>
+    <t>Rent and PC doc GUI functionality</t>
+  </si>
+  <si>
+    <t>08.06 || 11:00</t>
+  </si>
+  <si>
+    <t>Restock of stores</t>
+  </si>
+  <si>
+    <t>11.06 || 10:00</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1572,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1577,7 +1607,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1788,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,7 +1894,7 @@
       </c>
       <c r="M2" s="17" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>24%</v>
+        <v>23%</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>15</v>
@@ -1900,11 +1930,11 @@
       </c>
       <c r="K3" s="16">
         <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>3591</v>
+        <v>3711</v>
       </c>
       <c r="L3" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>59:51</v>
+        <v>61:51</v>
       </c>
       <c r="M3" s="17" t="str">
         <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
@@ -1949,11 +1979,11 @@
       </c>
       <c r="K4" s="16">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>4496</v>
+        <v>4676</v>
       </c>
       <c r="L4" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>74:56</v>
+        <v>77:56</v>
       </c>
       <c r="M4" s="17" t="str">
         <f>ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
@@ -1965,7 +1995,7 @@
       <c r="P4" s="27"/>
       <c r="Q4" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;Q$2&amp;"*"))</f>
-        <v>3591</v>
+        <v>3711</v>
       </c>
       <c r="R4" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O4&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
@@ -2002,7 +2032,7 @@
       </c>
       <c r="M5" s="17" t="str">
         <f>ROUND((K5) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>21%</v>
+        <v>20%</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>7</v>
@@ -2011,7 +2041,7 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="40">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;R$2&amp;"*"))</f>
-        <v>4496</v>
+        <v>4676</v>
       </c>
       <c r="S5" s="34">
         <f>(SUMIFS($D:$D,$B:$B, "*"&amp;$O5&amp;"*",$B:$B,"*"&amp;S$2&amp;"*"))</f>
@@ -2045,7 +2075,7 @@
       </c>
       <c r="M6" s="21" t="str">
         <f>ROUND(($K$6) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>7%</v>
+        <v>6%</v>
       </c>
       <c r="O6" s="29" t="s">
         <v>13</v>
@@ -2076,11 +2106,11 @@
       </c>
       <c r="K7" s="16">
         <f>SUM(K2:K5)</f>
-        <v>14557</v>
+        <v>14857</v>
       </c>
       <c r="L7" s="72" t="str">
         <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
-        <v>242:37</v>
+        <v>247:37</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3981,34 +4011,74 @@
       </c>
     </row>
     <row r="141" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="6"/>
-      <c r="B141" s="6"/>
-      <c r="C141" s="38"/>
-      <c r="D141" s="6"/>
+      <c r="A141" s="64" t="s">
+        <v>246</v>
+      </c>
+      <c r="B141" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C141" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="D141" s="64">
+        <v>30</v>
+      </c>
     </row>
     <row r="142" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="6"/>
-      <c r="B142" s="6"/>
-      <c r="C142" s="38"/>
-      <c r="D142" s="6"/>
+      <c r="A142" s="64" t="s">
+        <v>248</v>
+      </c>
+      <c r="B142" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="D142" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="143" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="6"/>
-      <c r="B143" s="6"/>
-      <c r="C143" s="38"/>
-      <c r="D143" s="6"/>
+      <c r="A143" s="64" t="s">
+        <v>250</v>
+      </c>
+      <c r="B143" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" s="70" t="s">
+        <v>251</v>
+      </c>
+      <c r="D143" s="64">
+        <v>30</v>
+      </c>
     </row>
     <row r="144" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="6"/>
-      <c r="B144" s="6"/>
-      <c r="C144" s="38"/>
-      <c r="D144" s="6"/>
+      <c r="A144" s="64" t="s">
+        <v>252</v>
+      </c>
+      <c r="B144" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144" s="70" t="s">
+        <v>253</v>
+      </c>
+      <c r="D144" s="64">
+        <v>120</v>
+      </c>
     </row>
     <row r="145" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="6"/>
-      <c r="B145" s="6"/>
-      <c r="C145" s="38"/>
-      <c r="D145" s="6"/>
+      <c r="A145" s="64" t="s">
+        <v>254</v>
+      </c>
+      <c r="B145" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" s="70" t="s">
+        <v>255</v>
+      </c>
+      <c r="D145" s="64">
+        <v>60</v>
+      </c>
     </row>
     <row r="146" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="6"/>

</xml_diff>